<commit_message>
bug screen shot added
</commit_message>
<xml_diff>
--- a/Rokomari_Signup.xlsx
+++ b/Rokomari_Signup.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>TC-7</t>
+  </si>
+  <si>
+    <t>Click Here</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1403,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1969,13 +1972,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1988,19 +1988,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2011,130 +2020,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2163,41 +2052,148 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2208,11 +2204,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2229,17 +2220,32 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2425,7 +2431,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2664,9 +2670,9 @@
   </sheetPr>
   <dimension ref="A1:AC1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2688,16 +2694,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="192" customFormat="1" ht="15" customHeight="1">
-      <c r="F1" s="267" t="s">
+      <c r="F1" s="223" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="268"/>
+      <c r="G1" s="224"/>
     </row>
     <row r="2" spans="1:29" s="192" customFormat="1" ht="15" customHeight="1">
-      <c r="D2" s="265" t="s">
+      <c r="D2" s="221" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="266"/>
+      <c r="E2" s="222"/>
     </row>
     <row r="3" spans="1:29" s="192" customFormat="1" ht="15" customHeight="1">
       <c r="D3" s="199" t="s">
@@ -2991,36 +2997,36 @@
       <c r="AC10" s="205"/>
     </row>
     <row r="11" spans="1:29" ht="30" customHeight="1">
-      <c r="A11" s="215" t="s">
+      <c r="A11" s="214" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="284" t="s">
+      <c r="B11" s="217" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="286" t="s">
+      <c r="C11" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="218" t="s">
+      <c r="D11" s="212" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="220" t="s">
+      <c r="E11" s="240" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="258" t="s">
+      <c r="F11" s="261" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="220" t="s">
+      <c r="G11" s="240" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="220" t="s">
+      <c r="H11" s="240" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="277" t="s">
+      <c r="I11" s="237" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="271"/>
-      <c r="K11" s="274"/>
-      <c r="L11" s="223" t="s">
+      <c r="J11" s="231"/>
+      <c r="K11" s="234"/>
+      <c r="L11" s="225" t="s">
         <v>85</v>
       </c>
       <c r="M11" s="198"/>
@@ -3042,18 +3048,18 @@
       <c r="AC11" s="4"/>
     </row>
     <row r="12" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A12" s="216"/>
-      <c r="B12" s="285"/>
-      <c r="C12" s="287"/>
-      <c r="D12" s="283"/>
-      <c r="E12" s="280"/>
-      <c r="F12" s="259"/>
-      <c r="G12" s="221"/>
-      <c r="H12" s="280"/>
-      <c r="I12" s="278"/>
-      <c r="J12" s="272"/>
-      <c r="K12" s="275"/>
-      <c r="L12" s="224"/>
+      <c r="A12" s="215"/>
+      <c r="B12" s="218"/>
+      <c r="C12" s="220"/>
+      <c r="D12" s="213"/>
+      <c r="E12" s="241"/>
+      <c r="F12" s="262"/>
+      <c r="G12" s="243"/>
+      <c r="H12" s="241"/>
+      <c r="I12" s="238"/>
+      <c r="J12" s="232"/>
+      <c r="K12" s="235"/>
+      <c r="L12" s="226"/>
       <c r="M12" s="197"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -3073,18 +3079,18 @@
       <c r="AC12" s="4"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A13" s="216"/>
-      <c r="B13" s="285"/>
-      <c r="C13" s="287"/>
-      <c r="D13" s="283"/>
-      <c r="E13" s="280"/>
-      <c r="F13" s="259"/>
-      <c r="G13" s="221"/>
-      <c r="H13" s="280"/>
-      <c r="I13" s="278"/>
-      <c r="J13" s="272"/>
-      <c r="K13" s="275"/>
-      <c r="L13" s="224"/>
+      <c r="A13" s="215"/>
+      <c r="B13" s="218"/>
+      <c r="C13" s="220"/>
+      <c r="D13" s="213"/>
+      <c r="E13" s="241"/>
+      <c r="F13" s="262"/>
+      <c r="G13" s="243"/>
+      <c r="H13" s="241"/>
+      <c r="I13" s="238"/>
+      <c r="J13" s="232"/>
+      <c r="K13" s="235"/>
+      <c r="L13" s="226"/>
       <c r="M13" s="190"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -3104,18 +3110,18 @@
       <c r="AC13" s="4"/>
     </row>
     <row r="14" spans="1:29" ht="25.5" customHeight="1">
-      <c r="A14" s="216"/>
-      <c r="B14" s="285"/>
-      <c r="C14" s="287"/>
-      <c r="D14" s="283"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="259"/>
-      <c r="G14" s="221"/>
-      <c r="H14" s="280"/>
-      <c r="I14" s="278"/>
-      <c r="J14" s="272"/>
-      <c r="K14" s="275"/>
-      <c r="L14" s="224"/>
+      <c r="A14" s="215"/>
+      <c r="B14" s="218"/>
+      <c r="C14" s="220"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="241"/>
+      <c r="F14" s="262"/>
+      <c r="G14" s="243"/>
+      <c r="H14" s="241"/>
+      <c r="I14" s="238"/>
+      <c r="J14" s="232"/>
+      <c r="K14" s="235"/>
+      <c r="L14" s="226"/>
       <c r="M14" s="190"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -3135,18 +3141,18 @@
       <c r="AC14" s="4"/>
     </row>
     <row r="15" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A15" s="216"/>
-      <c r="B15" s="285"/>
-      <c r="C15" s="287"/>
-      <c r="D15" s="283"/>
-      <c r="E15" s="280"/>
-      <c r="F15" s="259"/>
-      <c r="G15" s="221"/>
-      <c r="H15" s="280"/>
-      <c r="I15" s="278"/>
-      <c r="J15" s="272"/>
-      <c r="K15" s="275"/>
-      <c r="L15" s="224"/>
+      <c r="A15" s="215"/>
+      <c r="B15" s="218"/>
+      <c r="C15" s="220"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="241"/>
+      <c r="F15" s="262"/>
+      <c r="G15" s="243"/>
+      <c r="H15" s="241"/>
+      <c r="I15" s="238"/>
+      <c r="J15" s="232"/>
+      <c r="K15" s="235"/>
+      <c r="L15" s="226"/>
       <c r="M15" s="190"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -3166,18 +3172,18 @@
       <c r="AC15" s="4"/>
     </row>
     <row r="16" spans="1:29" s="189" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="216"/>
-      <c r="B16" s="285"/>
-      <c r="C16" s="287"/>
-      <c r="D16" s="283"/>
-      <c r="E16" s="280"/>
-      <c r="F16" s="259"/>
-      <c r="G16" s="221"/>
-      <c r="H16" s="280"/>
-      <c r="I16" s="278"/>
-      <c r="J16" s="272"/>
-      <c r="K16" s="275"/>
-      <c r="L16" s="224"/>
+      <c r="A16" s="215"/>
+      <c r="B16" s="218"/>
+      <c r="C16" s="220"/>
+      <c r="D16" s="213"/>
+      <c r="E16" s="241"/>
+      <c r="F16" s="262"/>
+      <c r="G16" s="243"/>
+      <c r="H16" s="241"/>
+      <c r="I16" s="238"/>
+      <c r="J16" s="232"/>
+      <c r="K16" s="235"/>
+      <c r="L16" s="226"/>
       <c r="M16" s="190"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -3197,18 +3203,18 @@
       <c r="AC16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A17" s="217"/>
-      <c r="B17" s="285"/>
-      <c r="C17" s="287"/>
-      <c r="D17" s="283"/>
-      <c r="E17" s="281"/>
-      <c r="F17" s="260"/>
-      <c r="G17" s="222"/>
-      <c r="H17" s="281"/>
-      <c r="I17" s="279"/>
-      <c r="J17" s="273"/>
-      <c r="K17" s="276"/>
-      <c r="L17" s="225"/>
+      <c r="A17" s="216"/>
+      <c r="B17" s="218"/>
+      <c r="C17" s="220"/>
+      <c r="D17" s="213"/>
+      <c r="E17" s="242"/>
+      <c r="F17" s="263"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="242"/>
+      <c r="I17" s="239"/>
+      <c r="J17" s="233"/>
+      <c r="K17" s="236"/>
+      <c r="L17" s="227"/>
       <c r="M17" s="191"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -3233,7 +3239,7 @@
       </c>
       <c r="B18" s="194"/>
       <c r="C18" s="134"/>
-      <c r="D18" s="231" t="s">
+      <c r="D18" s="279" t="s">
         <v>89</v>
       </c>
       <c r="E18" s="195" t="s">
@@ -3275,30 +3281,32 @@
       <c r="AC18" s="4"/>
     </row>
     <row r="19" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A19" s="223" t="s">
+      <c r="A19" s="225" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="231"/>
-      <c r="C19" s="224"/>
-      <c r="D19" s="231"/>
-      <c r="E19" s="221" t="s">
+      <c r="B19" s="279"/>
+      <c r="C19" s="226"/>
+      <c r="D19" s="279"/>
+      <c r="E19" s="243" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="234" t="s">
+      <c r="F19" s="283" t="s">
         <v>95</v>
       </c>
-      <c r="G19" s="236" t="s">
+      <c r="G19" s="274" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="221" t="s">
+      <c r="H19" s="243" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="221" t="s">
+      <c r="I19" s="243" t="s">
         <v>100</v>
       </c>
-      <c r="J19" s="261"/>
-      <c r="K19" s="221"/>
-      <c r="L19" s="224" t="s">
+      <c r="J19" s="315" t="s">
+        <v>122</v>
+      </c>
+      <c r="K19" s="243"/>
+      <c r="L19" s="226" t="s">
         <v>99</v>
       </c>
       <c r="M19" s="29"/>
@@ -3320,18 +3328,18 @@
       <c r="AC19" s="4"/>
     </row>
     <row r="20" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A20" s="224"/>
-      <c r="B20" s="231"/>
-      <c r="C20" s="224"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="221"/>
-      <c r="F20" s="234"/>
-      <c r="G20" s="237"/>
-      <c r="H20" s="221"/>
-      <c r="I20" s="221"/>
-      <c r="J20" s="261"/>
-      <c r="K20" s="221"/>
-      <c r="L20" s="224"/>
+      <c r="A20" s="226"/>
+      <c r="B20" s="279"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="279"/>
+      <c r="E20" s="243"/>
+      <c r="F20" s="283"/>
+      <c r="G20" s="275"/>
+      <c r="H20" s="243"/>
+      <c r="I20" s="243"/>
+      <c r="J20" s="315"/>
+      <c r="K20" s="243"/>
+      <c r="L20" s="226"/>
       <c r="M20" s="30"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -3351,18 +3359,18 @@
       <c r="AC20" s="4"/>
     </row>
     <row r="21" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A21" s="224"/>
-      <c r="B21" s="231"/>
-      <c r="C21" s="224"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="221"/>
-      <c r="F21" s="234"/>
-      <c r="G21" s="237"/>
-      <c r="H21" s="221"/>
-      <c r="I21" s="221"/>
-      <c r="J21" s="261"/>
-      <c r="K21" s="221"/>
-      <c r="L21" s="224"/>
+      <c r="A21" s="226"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="226"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="243"/>
+      <c r="F21" s="283"/>
+      <c r="G21" s="275"/>
+      <c r="H21" s="243"/>
+      <c r="I21" s="243"/>
+      <c r="J21" s="315"/>
+      <c r="K21" s="243"/>
+      <c r="L21" s="226"/>
       <c r="M21" s="30"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -3382,18 +3390,18 @@
       <c r="AC21" s="4"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A22" s="224"/>
-      <c r="B22" s="231"/>
-      <c r="C22" s="224"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="221"/>
-      <c r="F22" s="234"/>
-      <c r="G22" s="237"/>
-      <c r="H22" s="221"/>
-      <c r="I22" s="221"/>
-      <c r="J22" s="261"/>
-      <c r="K22" s="221"/>
-      <c r="L22" s="224"/>
+      <c r="A22" s="226"/>
+      <c r="B22" s="279"/>
+      <c r="C22" s="226"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="243"/>
+      <c r="F22" s="283"/>
+      <c r="G22" s="275"/>
+      <c r="H22" s="243"/>
+      <c r="I22" s="243"/>
+      <c r="J22" s="315"/>
+      <c r="K22" s="243"/>
+      <c r="L22" s="226"/>
       <c r="M22" s="32"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -3413,18 +3421,18 @@
       <c r="AC22" s="4"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A23" s="224"/>
-      <c r="B23" s="231"/>
-      <c r="C23" s="224"/>
-      <c r="D23" s="231"/>
-      <c r="E23" s="221"/>
-      <c r="F23" s="234"/>
-      <c r="G23" s="237"/>
-      <c r="H23" s="221"/>
-      <c r="I23" s="221"/>
-      <c r="J23" s="261"/>
-      <c r="K23" s="221"/>
-      <c r="L23" s="224"/>
+      <c r="A23" s="226"/>
+      <c r="B23" s="279"/>
+      <c r="C23" s="226"/>
+      <c r="D23" s="279"/>
+      <c r="E23" s="243"/>
+      <c r="F23" s="283"/>
+      <c r="G23" s="275"/>
+      <c r="H23" s="243"/>
+      <c r="I23" s="243"/>
+      <c r="J23" s="315"/>
+      <c r="K23" s="243"/>
+      <c r="L23" s="226"/>
       <c r="M23" s="25"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -3444,18 +3452,18 @@
       <c r="AC23" s="4"/>
     </row>
     <row r="24" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A24" s="225"/>
-      <c r="B24" s="231"/>
-      <c r="C24" s="224"/>
-      <c r="D24" s="231"/>
-      <c r="E24" s="222"/>
-      <c r="F24" s="235"/>
-      <c r="G24" s="238"/>
-      <c r="H24" s="222"/>
-      <c r="I24" s="221"/>
-      <c r="J24" s="262"/>
-      <c r="K24" s="222"/>
-      <c r="L24" s="225"/>
+      <c r="A24" s="227"/>
+      <c r="B24" s="279"/>
+      <c r="C24" s="226"/>
+      <c r="D24" s="279"/>
+      <c r="E24" s="244"/>
+      <c r="F24" s="284"/>
+      <c r="G24" s="276"/>
+      <c r="H24" s="244"/>
+      <c r="I24" s="243"/>
+      <c r="J24" s="316"/>
+      <c r="K24" s="244"/>
+      <c r="L24" s="227"/>
       <c r="M24" s="25"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -3475,30 +3483,32 @@
       <c r="AC24" s="4"/>
     </row>
     <row r="25" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A25" s="215" t="s">
+      <c r="A25" s="214" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="226"/>
-      <c r="C25" s="226"/>
-      <c r="D25" s="231"/>
-      <c r="E25" s="227" t="s">
+      <c r="B25" s="282"/>
+      <c r="C25" s="282"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="248" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="227" t="s">
+      <c r="F25" s="248" t="s">
         <v>104</v>
       </c>
-      <c r="G25" s="230" t="s">
+      <c r="G25" s="264" t="s">
         <v>105</v>
       </c>
-      <c r="H25" s="230" t="s">
+      <c r="H25" s="264" t="s">
         <v>106</v>
       </c>
-      <c r="I25" s="221" t="s">
+      <c r="I25" s="243" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="212"/>
-      <c r="K25" s="212"/>
-      <c r="L25" s="223" t="s">
+      <c r="J25" s="317" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" s="245"/>
+      <c r="L25" s="225" t="s">
         <v>99</v>
       </c>
       <c r="M25" s="25"/>
@@ -3520,18 +3530,18 @@
       <c r="AC25" s="4"/>
     </row>
     <row r="26" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A26" s="216"/>
-      <c r="B26" s="226"/>
-      <c r="C26" s="226"/>
-      <c r="D26" s="231"/>
-      <c r="E26" s="228"/>
-      <c r="F26" s="228"/>
-      <c r="G26" s="232"/>
-      <c r="H26" s="263"/>
-      <c r="I26" s="221"/>
-      <c r="J26" s="213"/>
-      <c r="K26" s="213"/>
-      <c r="L26" s="224"/>
+      <c r="A26" s="215"/>
+      <c r="B26" s="282"/>
+      <c r="C26" s="282"/>
+      <c r="D26" s="279"/>
+      <c r="E26" s="249"/>
+      <c r="F26" s="249"/>
+      <c r="G26" s="280"/>
+      <c r="H26" s="265"/>
+      <c r="I26" s="243"/>
+      <c r="J26" s="315"/>
+      <c r="K26" s="246"/>
+      <c r="L26" s="226"/>
       <c r="M26" s="25"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -3551,18 +3561,18 @@
       <c r="AC26" s="4"/>
     </row>
     <row r="27" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A27" s="216"/>
-      <c r="B27" s="226"/>
-      <c r="C27" s="226"/>
-      <c r="D27" s="231"/>
-      <c r="E27" s="228"/>
-      <c r="F27" s="228"/>
-      <c r="G27" s="232"/>
-      <c r="H27" s="263"/>
-      <c r="I27" s="221"/>
-      <c r="J27" s="213"/>
-      <c r="K27" s="213"/>
-      <c r="L27" s="224"/>
+      <c r="A27" s="215"/>
+      <c r="B27" s="282"/>
+      <c r="C27" s="282"/>
+      <c r="D27" s="279"/>
+      <c r="E27" s="249"/>
+      <c r="F27" s="249"/>
+      <c r="G27" s="280"/>
+      <c r="H27" s="265"/>
+      <c r="I27" s="243"/>
+      <c r="J27" s="315"/>
+      <c r="K27" s="246"/>
+      <c r="L27" s="226"/>
       <c r="M27" s="25"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -3582,18 +3592,18 @@
       <c r="AC27" s="4"/>
     </row>
     <row r="28" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A28" s="216"/>
-      <c r="B28" s="226"/>
-      <c r="C28" s="226"/>
-      <c r="D28" s="231"/>
-      <c r="E28" s="228"/>
-      <c r="F28" s="228"/>
-      <c r="G28" s="232"/>
-      <c r="H28" s="263"/>
-      <c r="I28" s="221"/>
-      <c r="J28" s="213"/>
-      <c r="K28" s="213"/>
-      <c r="L28" s="224"/>
+      <c r="A28" s="215"/>
+      <c r="B28" s="282"/>
+      <c r="C28" s="282"/>
+      <c r="D28" s="279"/>
+      <c r="E28" s="249"/>
+      <c r="F28" s="249"/>
+      <c r="G28" s="280"/>
+      <c r="H28" s="265"/>
+      <c r="I28" s="243"/>
+      <c r="J28" s="315"/>
+      <c r="K28" s="246"/>
+      <c r="L28" s="226"/>
       <c r="M28" s="25"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -3613,18 +3623,18 @@
       <c r="AC28" s="4"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A29" s="216"/>
-      <c r="B29" s="226"/>
-      <c r="C29" s="226"/>
-      <c r="D29" s="231"/>
-      <c r="E29" s="228"/>
-      <c r="F29" s="228"/>
-      <c r="G29" s="232"/>
-      <c r="H29" s="263"/>
-      <c r="I29" s="221"/>
-      <c r="J29" s="213"/>
-      <c r="K29" s="213"/>
-      <c r="L29" s="224"/>
+      <c r="A29" s="215"/>
+      <c r="B29" s="282"/>
+      <c r="C29" s="282"/>
+      <c r="D29" s="279"/>
+      <c r="E29" s="249"/>
+      <c r="F29" s="249"/>
+      <c r="G29" s="280"/>
+      <c r="H29" s="265"/>
+      <c r="I29" s="243"/>
+      <c r="J29" s="315"/>
+      <c r="K29" s="246"/>
+      <c r="L29" s="226"/>
       <c r="M29" s="25"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -3644,18 +3654,18 @@
       <c r="AC29" s="4"/>
     </row>
     <row r="30" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A30" s="216"/>
-      <c r="B30" s="226"/>
-      <c r="C30" s="226"/>
-      <c r="D30" s="231"/>
-      <c r="E30" s="228"/>
-      <c r="F30" s="228"/>
-      <c r="G30" s="232"/>
-      <c r="H30" s="263"/>
-      <c r="I30" s="221"/>
-      <c r="J30" s="213"/>
-      <c r="K30" s="213"/>
-      <c r="L30" s="224"/>
+      <c r="A30" s="215"/>
+      <c r="B30" s="282"/>
+      <c r="C30" s="282"/>
+      <c r="D30" s="279"/>
+      <c r="E30" s="249"/>
+      <c r="F30" s="249"/>
+      <c r="G30" s="280"/>
+      <c r="H30" s="265"/>
+      <c r="I30" s="243"/>
+      <c r="J30" s="315"/>
+      <c r="K30" s="246"/>
+      <c r="L30" s="226"/>
       <c r="M30" s="25"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -3675,18 +3685,18 @@
       <c r="AC30" s="4"/>
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A31" s="217"/>
-      <c r="B31" s="226"/>
-      <c r="C31" s="226"/>
-      <c r="D31" s="231"/>
-      <c r="E31" s="229"/>
-      <c r="F31" s="229"/>
-      <c r="G31" s="233"/>
-      <c r="H31" s="264"/>
-      <c r="I31" s="222"/>
-      <c r="J31" s="214"/>
-      <c r="K31" s="214"/>
-      <c r="L31" s="225"/>
+      <c r="A31" s="216"/>
+      <c r="B31" s="282"/>
+      <c r="C31" s="282"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="250"/>
+      <c r="F31" s="250"/>
+      <c r="G31" s="281"/>
+      <c r="H31" s="266"/>
+      <c r="I31" s="244"/>
+      <c r="J31" s="316"/>
+      <c r="K31" s="247"/>
+      <c r="L31" s="227"/>
       <c r="M31" s="25"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -3706,32 +3716,32 @@
       <c r="AC31" s="4"/>
     </row>
     <row r="32" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A32" s="215" t="s">
+      <c r="A32" s="214" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="226"/>
-      <c r="C32" s="226"/>
-      <c r="D32" s="219" t="s">
+      <c r="B32" s="282"/>
+      <c r="C32" s="282"/>
+      <c r="D32" s="285" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="227" t="s">
+      <c r="E32" s="248" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="227" t="s">
+      <c r="F32" s="248" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="230" t="s">
+      <c r="G32" s="264" t="s">
         <v>112</v>
       </c>
-      <c r="H32" s="227" t="s">
+      <c r="H32" s="248" t="s">
         <v>113</v>
       </c>
-      <c r="I32" s="282" t="s">
+      <c r="I32" s="251" t="s">
         <v>114</v>
       </c>
-      <c r="J32" s="212"/>
-      <c r="K32" s="212"/>
-      <c r="L32" s="215" t="s">
+      <c r="J32" s="245"/>
+      <c r="K32" s="245"/>
+      <c r="L32" s="214" t="s">
         <v>85</v>
       </c>
       <c r="M32" s="25"/>
@@ -3753,18 +3763,18 @@
       <c r="AC32" s="4"/>
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A33" s="216"/>
-      <c r="B33" s="226"/>
-      <c r="C33" s="226"/>
-      <c r="D33" s="219"/>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
-      <c r="G33" s="228"/>
-      <c r="H33" s="228"/>
-      <c r="I33" s="221"/>
-      <c r="J33" s="213"/>
-      <c r="K33" s="213"/>
-      <c r="L33" s="216"/>
+      <c r="A33" s="215"/>
+      <c r="B33" s="282"/>
+      <c r="C33" s="282"/>
+      <c r="D33" s="285"/>
+      <c r="E33" s="249"/>
+      <c r="F33" s="249"/>
+      <c r="G33" s="249"/>
+      <c r="H33" s="249"/>
+      <c r="I33" s="243"/>
+      <c r="J33" s="246"/>
+      <c r="K33" s="246"/>
+      <c r="L33" s="215"/>
       <c r="M33" s="25"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -3784,18 +3794,18 @@
       <c r="AC33" s="4"/>
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A34" s="216"/>
-      <c r="B34" s="226"/>
-      <c r="C34" s="226"/>
-      <c r="D34" s="219"/>
-      <c r="E34" s="228"/>
-      <c r="F34" s="228"/>
-      <c r="G34" s="228"/>
-      <c r="H34" s="228"/>
-      <c r="I34" s="221"/>
-      <c r="J34" s="213"/>
-      <c r="K34" s="213"/>
-      <c r="L34" s="216"/>
+      <c r="A34" s="215"/>
+      <c r="B34" s="282"/>
+      <c r="C34" s="282"/>
+      <c r="D34" s="285"/>
+      <c r="E34" s="249"/>
+      <c r="F34" s="249"/>
+      <c r="G34" s="249"/>
+      <c r="H34" s="249"/>
+      <c r="I34" s="243"/>
+      <c r="J34" s="246"/>
+      <c r="K34" s="246"/>
+      <c r="L34" s="215"/>
       <c r="M34" s="21"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -3815,18 +3825,18 @@
       <c r="AC34" s="4"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A35" s="216"/>
-      <c r="B35" s="226"/>
-      <c r="C35" s="226"/>
-      <c r="D35" s="219"/>
-      <c r="E35" s="228"/>
-      <c r="F35" s="228"/>
-      <c r="G35" s="228"/>
-      <c r="H35" s="228"/>
-      <c r="I35" s="221"/>
-      <c r="J35" s="213"/>
-      <c r="K35" s="213"/>
-      <c r="L35" s="216"/>
+      <c r="A35" s="215"/>
+      <c r="B35" s="282"/>
+      <c r="C35" s="282"/>
+      <c r="D35" s="285"/>
+      <c r="E35" s="249"/>
+      <c r="F35" s="249"/>
+      <c r="G35" s="249"/>
+      <c r="H35" s="249"/>
+      <c r="I35" s="243"/>
+      <c r="J35" s="246"/>
+      <c r="K35" s="246"/>
+      <c r="L35" s="215"/>
       <c r="M35" s="25"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -3846,18 +3856,18 @@
       <c r="AC35" s="4"/>
     </row>
     <row r="36" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A36" s="216"/>
-      <c r="B36" s="226"/>
-      <c r="C36" s="226"/>
-      <c r="D36" s="219"/>
-      <c r="E36" s="228"/>
-      <c r="F36" s="228"/>
-      <c r="G36" s="228"/>
-      <c r="H36" s="228"/>
-      <c r="I36" s="221"/>
-      <c r="J36" s="213"/>
-      <c r="K36" s="213"/>
-      <c r="L36" s="216"/>
+      <c r="A36" s="215"/>
+      <c r="B36" s="282"/>
+      <c r="C36" s="282"/>
+      <c r="D36" s="285"/>
+      <c r="E36" s="249"/>
+      <c r="F36" s="249"/>
+      <c r="G36" s="249"/>
+      <c r="H36" s="249"/>
+      <c r="I36" s="243"/>
+      <c r="J36" s="246"/>
+      <c r="K36" s="246"/>
+      <c r="L36" s="215"/>
       <c r="M36" s="25"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -3877,18 +3887,18 @@
       <c r="AC36" s="4"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A37" s="216"/>
-      <c r="B37" s="226"/>
-      <c r="C37" s="226"/>
-      <c r="D37" s="219"/>
-      <c r="E37" s="228"/>
-      <c r="F37" s="228"/>
-      <c r="G37" s="228"/>
-      <c r="H37" s="228"/>
-      <c r="I37" s="221"/>
-      <c r="J37" s="213"/>
-      <c r="K37" s="213"/>
-      <c r="L37" s="216"/>
+      <c r="A37" s="215"/>
+      <c r="B37" s="282"/>
+      <c r="C37" s="282"/>
+      <c r="D37" s="285"/>
+      <c r="E37" s="249"/>
+      <c r="F37" s="249"/>
+      <c r="G37" s="249"/>
+      <c r="H37" s="249"/>
+      <c r="I37" s="243"/>
+      <c r="J37" s="246"/>
+      <c r="K37" s="246"/>
+      <c r="L37" s="215"/>
       <c r="M37" s="25"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
@@ -3908,18 +3918,18 @@
       <c r="AC37" s="4"/>
     </row>
     <row r="38" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A38" s="217"/>
-      <c r="B38" s="226"/>
-      <c r="C38" s="226"/>
-      <c r="D38" s="219"/>
-      <c r="E38" s="229"/>
-      <c r="F38" s="229"/>
-      <c r="G38" s="229"/>
-      <c r="H38" s="229"/>
-      <c r="I38" s="222"/>
-      <c r="J38" s="214"/>
-      <c r="K38" s="214"/>
-      <c r="L38" s="217"/>
+      <c r="A38" s="216"/>
+      <c r="B38" s="282"/>
+      <c r="C38" s="282"/>
+      <c r="D38" s="285"/>
+      <c r="E38" s="250"/>
+      <c r="F38" s="250"/>
+      <c r="G38" s="250"/>
+      <c r="H38" s="250"/>
+      <c r="I38" s="244"/>
+      <c r="J38" s="247"/>
+      <c r="K38" s="247"/>
+      <c r="L38" s="216"/>
       <c r="M38" s="25"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -3939,30 +3949,30 @@
       <c r="AC38" s="4"/>
     </row>
     <row r="39" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A39" s="218" t="s">
+      <c r="A39" s="212" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="226"/>
-      <c r="C39" s="226"/>
-      <c r="D39" s="219"/>
-      <c r="E39" s="220" t="s">
+      <c r="B39" s="282"/>
+      <c r="C39" s="282"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="220" t="s">
+      <c r="F39" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="G39" s="220" t="s">
+      <c r="G39" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="H39" s="220" t="s">
+      <c r="H39" s="240" t="s">
         <v>119</v>
       </c>
-      <c r="I39" s="220" t="s">
+      <c r="I39" s="240" t="s">
         <v>120</v>
       </c>
-      <c r="J39" s="212"/>
-      <c r="K39" s="212"/>
-      <c r="L39" s="223" t="s">
+      <c r="J39" s="245"/>
+      <c r="K39" s="245"/>
+      <c r="L39" s="225" t="s">
         <v>85</v>
       </c>
       <c r="M39" s="29"/>
@@ -3984,18 +3994,18 @@
       <c r="AC39" s="4"/>
     </row>
     <row r="40" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A40" s="216"/>
-      <c r="B40" s="226"/>
-      <c r="C40" s="226"/>
-      <c r="D40" s="219"/>
-      <c r="E40" s="221"/>
-      <c r="F40" s="221"/>
-      <c r="G40" s="221"/>
-      <c r="H40" s="221"/>
-      <c r="I40" s="221"/>
-      <c r="J40" s="213"/>
-      <c r="K40" s="213"/>
-      <c r="L40" s="224"/>
+      <c r="A40" s="215"/>
+      <c r="B40" s="282"/>
+      <c r="C40" s="282"/>
+      <c r="D40" s="285"/>
+      <c r="E40" s="243"/>
+      <c r="F40" s="243"/>
+      <c r="G40" s="243"/>
+      <c r="H40" s="243"/>
+      <c r="I40" s="243"/>
+      <c r="J40" s="246"/>
+      <c r="K40" s="246"/>
+      <c r="L40" s="226"/>
       <c r="M40" s="30"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
@@ -4015,18 +4025,18 @@
       <c r="AC40" s="4"/>
     </row>
     <row r="41" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A41" s="216"/>
-      <c r="B41" s="226"/>
-      <c r="C41" s="226"/>
-      <c r="D41" s="219"/>
-      <c r="E41" s="221"/>
-      <c r="F41" s="221"/>
-      <c r="G41" s="221"/>
-      <c r="H41" s="221"/>
-      <c r="I41" s="221"/>
-      <c r="J41" s="213"/>
-      <c r="K41" s="213"/>
-      <c r="L41" s="224"/>
+      <c r="A41" s="215"/>
+      <c r="B41" s="282"/>
+      <c r="C41" s="282"/>
+      <c r="D41" s="285"/>
+      <c r="E41" s="243"/>
+      <c r="F41" s="243"/>
+      <c r="G41" s="243"/>
+      <c r="H41" s="243"/>
+      <c r="I41" s="243"/>
+      <c r="J41" s="246"/>
+      <c r="K41" s="246"/>
+      <c r="L41" s="226"/>
       <c r="M41" s="30"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -4046,18 +4056,18 @@
       <c r="AC41" s="4"/>
     </row>
     <row r="42" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A42" s="216"/>
-      <c r="B42" s="226"/>
-      <c r="C42" s="226"/>
-      <c r="D42" s="219"/>
-      <c r="E42" s="221"/>
-      <c r="F42" s="221"/>
-      <c r="G42" s="221"/>
-      <c r="H42" s="221"/>
-      <c r="I42" s="221"/>
-      <c r="J42" s="213"/>
-      <c r="K42" s="213"/>
-      <c r="L42" s="224"/>
+      <c r="A42" s="215"/>
+      <c r="B42" s="282"/>
+      <c r="C42" s="282"/>
+      <c r="D42" s="285"/>
+      <c r="E42" s="243"/>
+      <c r="F42" s="243"/>
+      <c r="G42" s="243"/>
+      <c r="H42" s="243"/>
+      <c r="I42" s="243"/>
+      <c r="J42" s="246"/>
+      <c r="K42" s="246"/>
+      <c r="L42" s="226"/>
       <c r="M42" s="30"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
@@ -4077,18 +4087,18 @@
       <c r="AC42" s="4"/>
     </row>
     <row r="43" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A43" s="216"/>
-      <c r="B43" s="226"/>
-      <c r="C43" s="226"/>
-      <c r="D43" s="219"/>
-      <c r="E43" s="221"/>
-      <c r="F43" s="221"/>
-      <c r="G43" s="221"/>
-      <c r="H43" s="221"/>
-      <c r="I43" s="221"/>
-      <c r="J43" s="213"/>
-      <c r="K43" s="213"/>
-      <c r="L43" s="224"/>
+      <c r="A43" s="215"/>
+      <c r="B43" s="282"/>
+      <c r="C43" s="282"/>
+      <c r="D43" s="285"/>
+      <c r="E43" s="243"/>
+      <c r="F43" s="243"/>
+      <c r="G43" s="243"/>
+      <c r="H43" s="243"/>
+      <c r="I43" s="243"/>
+      <c r="J43" s="246"/>
+      <c r="K43" s="246"/>
+      <c r="L43" s="226"/>
       <c r="M43" s="30"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -4108,18 +4118,18 @@
       <c r="AC43" s="4"/>
     </row>
     <row r="44" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A44" s="217"/>
-      <c r="B44" s="226"/>
-      <c r="C44" s="226"/>
-      <c r="D44" s="219"/>
-      <c r="E44" s="221"/>
-      <c r="F44" s="221"/>
-      <c r="G44" s="222"/>
-      <c r="H44" s="222"/>
-      <c r="I44" s="222"/>
-      <c r="J44" s="214"/>
-      <c r="K44" s="214"/>
-      <c r="L44" s="225"/>
+      <c r="A44" s="216"/>
+      <c r="B44" s="282"/>
+      <c r="C44" s="282"/>
+      <c r="D44" s="285"/>
+      <c r="E44" s="243"/>
+      <c r="F44" s="243"/>
+      <c r="G44" s="244"/>
+      <c r="H44" s="244"/>
+      <c r="I44" s="244"/>
+      <c r="J44" s="247"/>
+      <c r="K44" s="247"/>
+      <c r="L44" s="227"/>
       <c r="M44" s="32"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -4139,7 +4149,7 @@
       <c r="AC44" s="4"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A45" s="215" t="s">
+      <c r="A45" s="214" t="s">
         <v>121</v>
       </c>
       <c r="B45" s="187"/>
@@ -4172,7 +4182,7 @@
       <c r="AC45" s="4"/>
     </row>
     <row r="46" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A46" s="216"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="187"/>
       <c r="C46" s="190"/>
       <c r="D46" s="190"/>
@@ -4203,7 +4213,7 @@
       <c r="AC46" s="4"/>
     </row>
     <row r="47" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A47" s="216"/>
+      <c r="A47" s="215"/>
       <c r="B47" s="187"/>
       <c r="C47" s="190"/>
       <c r="D47" s="46"/>
@@ -4234,7 +4244,7 @@
       <c r="AC47" s="4"/>
     </row>
     <row r="48" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A48" s="216"/>
+      <c r="A48" s="215"/>
       <c r="B48" s="187"/>
       <c r="C48" s="190"/>
       <c r="D48" s="46"/>
@@ -4265,7 +4275,7 @@
       <c r="AC48" s="4"/>
     </row>
     <row r="49" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A49" s="216"/>
+      <c r="A49" s="215"/>
       <c r="B49" s="187"/>
       <c r="C49" s="190"/>
       <c r="D49" s="46"/>
@@ -4296,7 +4306,7 @@
       <c r="AC49" s="4"/>
     </row>
     <row r="50" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A50" s="217"/>
+      <c r="A50" s="216"/>
       <c r="B50" s="187"/>
       <c r="C50" s="190"/>
       <c r="D50" s="47"/>
@@ -4332,7 +4342,7 @@
       </c>
       <c r="B51" s="187"/>
       <c r="C51" s="190"/>
-      <c r="D51" s="247"/>
+      <c r="D51" s="269"/>
       <c r="E51" s="49"/>
       <c r="F51" s="23"/>
       <c r="G51" s="23"/>
@@ -4365,7 +4375,7 @@
       </c>
       <c r="B52" s="187"/>
       <c r="C52" s="190"/>
-      <c r="D52" s="248"/>
+      <c r="D52" s="229"/>
       <c r="E52" s="49"/>
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
@@ -4398,7 +4408,7 @@
       </c>
       <c r="B53" s="187"/>
       <c r="C53" s="190"/>
-      <c r="D53" s="248"/>
+      <c r="D53" s="229"/>
       <c r="E53" s="53"/>
       <c r="F53" s="54"/>
       <c r="G53" s="55"/>
@@ -4431,7 +4441,7 @@
       </c>
       <c r="B54" s="187"/>
       <c r="C54" s="190"/>
-      <c r="D54" s="248"/>
+      <c r="D54" s="229"/>
       <c r="E54" s="58"/>
       <c r="F54" s="22"/>
       <c r="G54" s="38"/>
@@ -4464,7 +4474,7 @@
       </c>
       <c r="B55" s="187"/>
       <c r="C55" s="190"/>
-      <c r="D55" s="248"/>
+      <c r="D55" s="229"/>
       <c r="E55" s="58"/>
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
@@ -4497,7 +4507,7 @@
       </c>
       <c r="B56" s="187"/>
       <c r="C56" s="190"/>
-      <c r="D56" s="248"/>
+      <c r="D56" s="229"/>
       <c r="E56" s="58"/>
       <c r="F56" s="22"/>
       <c r="G56" s="55"/>
@@ -4530,7 +4540,7 @@
       </c>
       <c r="B57" s="187"/>
       <c r="C57" s="190"/>
-      <c r="D57" s="248"/>
+      <c r="D57" s="229"/>
       <c r="E57" s="49"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
@@ -4563,7 +4573,7 @@
       </c>
       <c r="B58" s="187"/>
       <c r="C58" s="190"/>
-      <c r="D58" s="248"/>
+      <c r="D58" s="229"/>
       <c r="E58" s="49"/>
       <c r="F58" s="16"/>
       <c r="G58" s="55"/>
@@ -4596,7 +4606,7 @@
       </c>
       <c r="B59" s="187"/>
       <c r="C59" s="190"/>
-      <c r="D59" s="248"/>
+      <c r="D59" s="229"/>
       <c r="E59" s="49"/>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
@@ -4629,7 +4639,7 @@
       </c>
       <c r="B60" s="187"/>
       <c r="C60" s="190"/>
-      <c r="D60" s="248"/>
+      <c r="D60" s="229"/>
       <c r="E60" s="49"/>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
@@ -4693,7 +4703,7 @@
       </c>
       <c r="B62" s="187"/>
       <c r="C62" s="190"/>
-      <c r="D62" s="249"/>
+      <c r="D62" s="252"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="55"/>
@@ -4726,7 +4736,7 @@
       </c>
       <c r="B63" s="187"/>
       <c r="C63" s="190"/>
-      <c r="D63" s="240"/>
+      <c r="D63" s="257"/>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
       <c r="G63" s="50"/>
@@ -4759,7 +4769,7 @@
       </c>
       <c r="B64" s="187"/>
       <c r="C64" s="190"/>
-      <c r="D64" s="240"/>
+      <c r="D64" s="257"/>
       <c r="E64" s="60"/>
       <c r="F64" s="61"/>
       <c r="G64" s="60"/>
@@ -4792,7 +4802,7 @@
       </c>
       <c r="B65" s="187"/>
       <c r="C65" s="190"/>
-      <c r="D65" s="240"/>
+      <c r="D65" s="257"/>
       <c r="E65" s="62"/>
       <c r="F65" s="63"/>
       <c r="G65" s="63"/>
@@ -4825,7 +4835,7 @@
       </c>
       <c r="B66" s="187"/>
       <c r="C66" s="190"/>
-      <c r="D66" s="241"/>
+      <c r="D66" s="253"/>
       <c r="E66" s="35"/>
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
@@ -4889,7 +4899,7 @@
       </c>
       <c r="B68" s="187"/>
       <c r="C68" s="190"/>
-      <c r="D68" s="249"/>
+      <c r="D68" s="252"/>
       <c r="E68" s="38"/>
       <c r="F68" s="22"/>
       <c r="G68" s="22"/>
@@ -4922,7 +4932,7 @@
       </c>
       <c r="B69" s="187"/>
       <c r="C69" s="190"/>
-      <c r="D69" s="240"/>
+      <c r="D69" s="257"/>
       <c r="E69" s="38"/>
       <c r="F69" s="22"/>
       <c r="G69" s="16"/>
@@ -4986,7 +4996,7 @@
       </c>
       <c r="B71" s="187"/>
       <c r="C71" s="190"/>
-      <c r="D71" s="250"/>
+      <c r="D71" s="270"/>
       <c r="E71" s="45"/>
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
@@ -5019,7 +5029,7 @@
       </c>
       <c r="B72" s="187"/>
       <c r="C72" s="190"/>
-      <c r="D72" s="240"/>
+      <c r="D72" s="257"/>
       <c r="E72" s="45"/>
       <c r="F72" s="16"/>
       <c r="G72" s="23"/>
@@ -5052,7 +5062,7 @@
       </c>
       <c r="B73" s="187"/>
       <c r="C73" s="190"/>
-      <c r="D73" s="240"/>
+      <c r="D73" s="257"/>
       <c r="E73" s="68"/>
       <c r="F73" s="69"/>
       <c r="G73" s="70"/>
@@ -5085,7 +5095,7 @@
       </c>
       <c r="B74" s="187"/>
       <c r="C74" s="190"/>
-      <c r="D74" s="240"/>
+      <c r="D74" s="257"/>
       <c r="E74" s="71"/>
       <c r="F74" s="22"/>
       <c r="G74" s="54"/>
@@ -5118,7 +5128,7 @@
       </c>
       <c r="B75" s="187"/>
       <c r="C75" s="190"/>
-      <c r="D75" s="240"/>
+      <c r="D75" s="257"/>
       <c r="E75" s="71"/>
       <c r="F75" s="22"/>
       <c r="G75" s="16"/>
@@ -5151,7 +5161,7 @@
       </c>
       <c r="B76" s="187"/>
       <c r="C76" s="190"/>
-      <c r="D76" s="240"/>
+      <c r="D76" s="257"/>
       <c r="E76" s="45"/>
       <c r="F76" s="16"/>
       <c r="G76" s="16"/>
@@ -5184,7 +5194,7 @@
       </c>
       <c r="B77" s="187"/>
       <c r="C77" s="190"/>
-      <c r="D77" s="240"/>
+      <c r="D77" s="257"/>
       <c r="E77" s="45"/>
       <c r="F77" s="16"/>
       <c r="G77" s="16"/>
@@ -5217,7 +5227,7 @@
       </c>
       <c r="B78" s="187"/>
       <c r="C78" s="190"/>
-      <c r="D78" s="240"/>
+      <c r="D78" s="257"/>
       <c r="E78" s="45"/>
       <c r="F78" s="16"/>
       <c r="G78" s="16"/>
@@ -5250,7 +5260,7 @@
       </c>
       <c r="B79" s="187"/>
       <c r="C79" s="190"/>
-      <c r="D79" s="240"/>
+      <c r="D79" s="257"/>
       <c r="E79" s="68"/>
       <c r="F79" s="69"/>
       <c r="G79" s="72"/>
@@ -5283,7 +5293,7 @@
       </c>
       <c r="B80" s="187"/>
       <c r="C80" s="190"/>
-      <c r="D80" s="240"/>
+      <c r="D80" s="257"/>
       <c r="E80" s="73"/>
       <c r="F80" s="74"/>
       <c r="G80" s="74"/>
@@ -5316,7 +5326,7 @@
       </c>
       <c r="B81" s="187"/>
       <c r="C81" s="190"/>
-      <c r="D81" s="240"/>
+      <c r="D81" s="257"/>
       <c r="E81" s="71"/>
       <c r="F81" s="22"/>
       <c r="G81" s="22"/>
@@ -5380,7 +5390,7 @@
       </c>
       <c r="B83" s="187"/>
       <c r="C83" s="190"/>
-      <c r="D83" s="251"/>
+      <c r="D83" s="271"/>
       <c r="E83" s="31"/>
       <c r="F83" s="16"/>
       <c r="G83" s="16"/>
@@ -5413,7 +5423,7 @@
       </c>
       <c r="B84" s="187"/>
       <c r="C84" s="190"/>
-      <c r="D84" s="248"/>
+      <c r="D84" s="229"/>
       <c r="E84" s="31"/>
       <c r="F84" s="16"/>
       <c r="G84" s="16"/>
@@ -5446,7 +5456,7 @@
       </c>
       <c r="B85" s="187"/>
       <c r="C85" s="190"/>
-      <c r="D85" s="248"/>
+      <c r="D85" s="229"/>
       <c r="E85" s="31"/>
       <c r="F85" s="23"/>
       <c r="G85" s="23"/>
@@ -5479,7 +5489,7 @@
       </c>
       <c r="B86" s="187"/>
       <c r="C86" s="190"/>
-      <c r="D86" s="248"/>
+      <c r="D86" s="229"/>
       <c r="E86" s="62"/>
       <c r="F86" s="35"/>
       <c r="G86" s="75"/>
@@ -5512,7 +5522,7 @@
       </c>
       <c r="B87" s="187"/>
       <c r="C87" s="190"/>
-      <c r="D87" s="248"/>
+      <c r="D87" s="229"/>
       <c r="E87" s="31"/>
       <c r="F87" s="16"/>
       <c r="G87" s="16"/>
@@ -5545,7 +5555,7 @@
       </c>
       <c r="B88" s="187"/>
       <c r="C88" s="190"/>
-      <c r="D88" s="248"/>
+      <c r="D88" s="229"/>
       <c r="E88" s="53"/>
       <c r="F88" s="54"/>
       <c r="G88" s="55"/>
@@ -5578,7 +5588,7 @@
       </c>
       <c r="B89" s="187"/>
       <c r="C89" s="190"/>
-      <c r="D89" s="248"/>
+      <c r="D89" s="229"/>
       <c r="E89" s="53"/>
       <c r="F89" s="22"/>
       <c r="G89" s="22"/>
@@ -5611,7 +5621,7 @@
       </c>
       <c r="B90" s="187"/>
       <c r="C90" s="190"/>
-      <c r="D90" s="248"/>
+      <c r="D90" s="229"/>
       <c r="E90" s="53"/>
       <c r="F90" s="22"/>
       <c r="G90" s="16"/>
@@ -5644,7 +5654,7 @@
       </c>
       <c r="B91" s="187"/>
       <c r="C91" s="190"/>
-      <c r="D91" s="248"/>
+      <c r="D91" s="229"/>
       <c r="E91" s="53"/>
       <c r="F91" s="38"/>
       <c r="G91" s="23"/>
@@ -5677,7 +5687,7 @@
       </c>
       <c r="B92" s="187"/>
       <c r="C92" s="190"/>
-      <c r="D92" s="248"/>
+      <c r="D92" s="229"/>
       <c r="E92" s="55"/>
       <c r="F92" s="33"/>
       <c r="G92" s="55"/>
@@ -5741,7 +5751,7 @@
       </c>
       <c r="B94" s="187"/>
       <c r="C94" s="190"/>
-      <c r="D94" s="246"/>
+      <c r="D94" s="256"/>
       <c r="E94" s="55"/>
       <c r="F94" s="56"/>
       <c r="G94" s="56"/>
@@ -5774,7 +5784,7 @@
       </c>
       <c r="B95" s="187"/>
       <c r="C95" s="190"/>
-      <c r="D95" s="240"/>
+      <c r="D95" s="257"/>
       <c r="E95" s="23"/>
       <c r="F95" s="16"/>
       <c r="G95" s="16"/>
@@ -5837,7 +5847,7 @@
       </c>
       <c r="B97" s="187"/>
       <c r="C97" s="190"/>
-      <c r="D97" s="245"/>
+      <c r="D97" s="268"/>
       <c r="E97" s="16"/>
       <c r="F97" s="16"/>
       <c r="G97" s="16"/>
@@ -5870,7 +5880,7 @@
       </c>
       <c r="B98" s="187"/>
       <c r="C98" s="190"/>
-      <c r="D98" s="240"/>
+      <c r="D98" s="257"/>
       <c r="E98" s="55"/>
       <c r="F98" s="56"/>
       <c r="G98" s="31"/>
@@ -5903,7 +5913,7 @@
       </c>
       <c r="B99" s="187"/>
       <c r="C99" s="190"/>
-      <c r="D99" s="240"/>
+      <c r="D99" s="257"/>
       <c r="E99" s="16"/>
       <c r="F99" s="16"/>
       <c r="G99" s="16"/>
@@ -5936,7 +5946,7 @@
       </c>
       <c r="B100" s="187"/>
       <c r="C100" s="190"/>
-      <c r="D100" s="240"/>
+      <c r="D100" s="257"/>
       <c r="E100" s="55"/>
       <c r="F100" s="56"/>
       <c r="G100" s="56"/>
@@ -5969,7 +5979,7 @@
       </c>
       <c r="B101" s="187"/>
       <c r="C101" s="190"/>
-      <c r="D101" s="240"/>
+      <c r="D101" s="257"/>
       <c r="E101" s="35"/>
       <c r="F101" s="35"/>
       <c r="G101" s="79"/>
@@ -6002,7 +6012,7 @@
       </c>
       <c r="B102" s="187"/>
       <c r="C102" s="190"/>
-      <c r="D102" s="240"/>
+      <c r="D102" s="257"/>
       <c r="E102" s="55"/>
       <c r="F102" s="56"/>
       <c r="G102" s="55"/>
@@ -6035,7 +6045,7 @@
       </c>
       <c r="B103" s="187"/>
       <c r="C103" s="190"/>
-      <c r="D103" s="241"/>
+      <c r="D103" s="253"/>
       <c r="E103" s="35"/>
       <c r="F103" s="35"/>
       <c r="G103" s="81"/>
@@ -6099,7 +6109,7 @@
       </c>
       <c r="B105" s="187"/>
       <c r="C105" s="190"/>
-      <c r="D105" s="269"/>
+      <c r="D105" s="228"/>
       <c r="E105" s="60"/>
       <c r="F105" s="87"/>
       <c r="G105" s="34"/>
@@ -6132,7 +6142,7 @@
       </c>
       <c r="B106" s="187"/>
       <c r="C106" s="190"/>
-      <c r="D106" s="248"/>
+      <c r="D106" s="229"/>
       <c r="E106" s="60"/>
       <c r="F106" s="35"/>
       <c r="G106" s="36"/>
@@ -6165,7 +6175,7 @@
       </c>
       <c r="B107" s="187"/>
       <c r="C107" s="190"/>
-      <c r="D107" s="248"/>
+      <c r="D107" s="229"/>
       <c r="E107" s="88"/>
       <c r="F107" s="37"/>
       <c r="G107" s="74"/>
@@ -6198,7 +6208,7 @@
       </c>
       <c r="B108" s="187"/>
       <c r="C108" s="190"/>
-      <c r="D108" s="248"/>
+      <c r="D108" s="229"/>
       <c r="E108" s="88"/>
       <c r="F108" s="37"/>
       <c r="G108" s="37"/>
@@ -6231,7 +6241,7 @@
       </c>
       <c r="B109" s="187"/>
       <c r="C109" s="190"/>
-      <c r="D109" s="248"/>
+      <c r="D109" s="229"/>
       <c r="E109" s="88"/>
       <c r="F109" s="37"/>
       <c r="G109" s="37"/>
@@ -6264,7 +6274,7 @@
       </c>
       <c r="B110" s="187"/>
       <c r="C110" s="190"/>
-      <c r="D110" s="248"/>
+      <c r="D110" s="229"/>
       <c r="E110" s="88"/>
       <c r="F110" s="37"/>
       <c r="G110" s="37"/>
@@ -6297,7 +6307,7 @@
       </c>
       <c r="B111" s="187"/>
       <c r="C111" s="190"/>
-      <c r="D111" s="248"/>
+      <c r="D111" s="229"/>
       <c r="E111" s="88"/>
       <c r="F111" s="37"/>
       <c r="G111" s="37"/>
@@ -6330,7 +6340,7 @@
       </c>
       <c r="B112" s="187"/>
       <c r="C112" s="190"/>
-      <c r="D112" s="248"/>
+      <c r="D112" s="229"/>
       <c r="E112" s="88"/>
       <c r="F112" s="37"/>
       <c r="G112" s="37"/>
@@ -6363,7 +6373,7 @@
       </c>
       <c r="B113" s="187"/>
       <c r="C113" s="190"/>
-      <c r="D113" s="270"/>
+      <c r="D113" s="230"/>
       <c r="E113" s="88"/>
       <c r="F113" s="37"/>
       <c r="G113" s="37"/>
@@ -6491,7 +6501,7 @@
       </c>
       <c r="B117" s="187"/>
       <c r="C117" s="32"/>
-      <c r="D117" s="249"/>
+      <c r="D117" s="252"/>
       <c r="E117" s="91"/>
       <c r="F117" s="91"/>
       <c r="G117" s="91"/>
@@ -6524,7 +6534,7 @@
       </c>
       <c r="B118" s="187"/>
       <c r="C118" s="32"/>
-      <c r="D118" s="241"/>
+      <c r="D118" s="253"/>
       <c r="E118" s="91"/>
       <c r="F118" s="91"/>
       <c r="G118" s="91"/>
@@ -7516,7 +7526,7 @@
       <c r="A150" s="99"/>
       <c r="B150" s="187"/>
       <c r="C150" s="32"/>
-      <c r="D150" s="252"/>
+      <c r="D150" s="272"/>
       <c r="E150" s="90"/>
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
@@ -7525,7 +7535,7 @@
       <c r="J150" s="37"/>
       <c r="K150" s="21"/>
       <c r="L150" s="28"/>
-      <c r="M150" s="256"/>
+      <c r="M150" s="258"/>
       <c r="N150" s="4"/>
       <c r="O150" s="4"/>
       <c r="P150" s="4"/>
@@ -7547,7 +7557,7 @@
       <c r="A151" s="20"/>
       <c r="B151" s="187"/>
       <c r="C151" s="32"/>
-      <c r="D151" s="240"/>
+      <c r="D151" s="257"/>
       <c r="E151" s="90"/>
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
@@ -7556,7 +7566,7 @@
       <c r="J151" s="37"/>
       <c r="K151" s="21"/>
       <c r="L151" s="28"/>
-      <c r="M151" s="240"/>
+      <c r="M151" s="257"/>
       <c r="N151" s="4"/>
       <c r="O151" s="4"/>
       <c r="P151" s="4"/>
@@ -7578,7 +7588,7 @@
       <c r="A152" s="20"/>
       <c r="B152" s="187"/>
       <c r="C152" s="32"/>
-      <c r="D152" s="240"/>
+      <c r="D152" s="257"/>
       <c r="E152" s="106"/>
       <c r="F152" s="30"/>
       <c r="G152" s="37"/>
@@ -7587,7 +7597,7 @@
       <c r="J152" s="37"/>
       <c r="K152" s="21"/>
       <c r="L152" s="28"/>
-      <c r="M152" s="240"/>
+      <c r="M152" s="257"/>
       <c r="N152" s="4"/>
       <c r="O152" s="4"/>
       <c r="P152" s="4"/>
@@ -7609,7 +7619,7 @@
       <c r="A153" s="20"/>
       <c r="B153" s="187"/>
       <c r="C153" s="32"/>
-      <c r="D153" s="240"/>
+      <c r="D153" s="257"/>
       <c r="E153" s="107"/>
       <c r="F153" s="103"/>
       <c r="G153" s="67"/>
@@ -7618,7 +7628,7 @@
       <c r="J153" s="37"/>
       <c r="K153" s="21"/>
       <c r="L153" s="28"/>
-      <c r="M153" s="240"/>
+      <c r="M153" s="257"/>
       <c r="N153" s="4"/>
       <c r="O153" s="4"/>
       <c r="P153" s="4"/>
@@ -7640,7 +7650,7 @@
       <c r="A154" s="20"/>
       <c r="B154" s="187"/>
       <c r="C154" s="32"/>
-      <c r="D154" s="240"/>
+      <c r="D154" s="257"/>
       <c r="E154" s="107"/>
       <c r="F154" s="103"/>
       <c r="G154" s="67"/>
@@ -7649,7 +7659,7 @@
       <c r="J154" s="37"/>
       <c r="K154" s="21"/>
       <c r="L154" s="28"/>
-      <c r="M154" s="240"/>
+      <c r="M154" s="257"/>
       <c r="N154" s="4"/>
       <c r="O154" s="4"/>
       <c r="P154" s="4"/>
@@ -7671,7 +7681,7 @@
       <c r="A155" s="20"/>
       <c r="B155" s="187"/>
       <c r="C155" s="32"/>
-      <c r="D155" s="240"/>
+      <c r="D155" s="257"/>
       <c r="E155" s="107"/>
       <c r="F155" s="103"/>
       <c r="G155" s="67"/>
@@ -7680,7 +7690,7 @@
       <c r="J155" s="37"/>
       <c r="K155" s="21"/>
       <c r="L155" s="28"/>
-      <c r="M155" s="240"/>
+      <c r="M155" s="257"/>
       <c r="N155" s="4"/>
       <c r="O155" s="4"/>
       <c r="P155" s="4"/>
@@ -7702,7 +7712,7 @@
       <c r="A156" s="20"/>
       <c r="B156" s="187"/>
       <c r="C156" s="32"/>
-      <c r="D156" s="240"/>
+      <c r="D156" s="257"/>
       <c r="E156" s="107"/>
       <c r="F156" s="103"/>
       <c r="G156" s="67"/>
@@ -7711,7 +7721,7 @@
       <c r="J156" s="37"/>
       <c r="K156" s="21"/>
       <c r="L156" s="28"/>
-      <c r="M156" s="240"/>
+      <c r="M156" s="257"/>
       <c r="N156" s="4"/>
       <c r="O156" s="4"/>
       <c r="P156" s="4"/>
@@ -7733,7 +7743,7 @@
       <c r="A157" s="20"/>
       <c r="B157" s="187"/>
       <c r="C157" s="32"/>
-      <c r="D157" s="240"/>
+      <c r="D157" s="257"/>
       <c r="E157" s="90"/>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
@@ -7742,7 +7752,7 @@
       <c r="J157" s="37"/>
       <c r="K157" s="21"/>
       <c r="L157" s="28"/>
-      <c r="M157" s="241"/>
+      <c r="M157" s="253"/>
       <c r="N157" s="4"/>
       <c r="O157" s="4"/>
       <c r="P157" s="4"/>
@@ -7764,7 +7774,7 @@
       <c r="A158" s="20"/>
       <c r="B158" s="187"/>
       <c r="C158" s="32"/>
-      <c r="D158" s="240"/>
+      <c r="D158" s="257"/>
       <c r="E158" s="90"/>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -7795,7 +7805,7 @@
       <c r="A159" s="20"/>
       <c r="B159" s="187"/>
       <c r="C159" s="32"/>
-      <c r="D159" s="240"/>
+      <c r="D159" s="257"/>
       <c r="E159" s="90"/>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -7826,7 +7836,7 @@
       <c r="A160" s="20"/>
       <c r="B160" s="188"/>
       <c r="C160" s="32"/>
-      <c r="D160" s="240"/>
+      <c r="D160" s="257"/>
       <c r="E160" s="90"/>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -7890,7 +7900,7 @@
       <c r="C162" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D162" s="253"/>
+      <c r="D162" s="273"/>
       <c r="E162" s="67"/>
       <c r="F162" s="37"/>
       <c r="G162" s="37"/>
@@ -7921,7 +7931,7 @@
       <c r="A163" s="20"/>
       <c r="B163" s="13"/>
       <c r="C163" s="109"/>
-      <c r="D163" s="240"/>
+      <c r="D163" s="257"/>
       <c r="E163" s="67"/>
       <c r="F163" s="37"/>
       <c r="G163" s="37"/>
@@ -7952,7 +7962,7 @@
       <c r="A164" s="20"/>
       <c r="B164" s="13"/>
       <c r="C164" s="109"/>
-      <c r="D164" s="240"/>
+      <c r="D164" s="257"/>
       <c r="E164" s="67"/>
       <c r="F164" s="37"/>
       <c r="G164" s="37"/>
@@ -7983,7 +7993,7 @@
       <c r="A165" s="20"/>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
-      <c r="D165" s="240"/>
+      <c r="D165" s="257"/>
       <c r="E165" s="110"/>
       <c r="F165" s="74"/>
       <c r="G165" s="37"/>
@@ -8014,7 +8024,7 @@
       <c r="A166" s="20"/>
       <c r="B166" s="28"/>
       <c r="C166" s="13"/>
-      <c r="D166" s="240"/>
+      <c r="D166" s="257"/>
       <c r="E166" s="110"/>
       <c r="F166" s="74"/>
       <c r="G166" s="37"/>
@@ -8045,7 +8055,7 @@
       <c r="A167" s="20"/>
       <c r="B167" s="28"/>
       <c r="C167" s="13"/>
-      <c r="D167" s="240"/>
+      <c r="D167" s="257"/>
       <c r="E167" s="110"/>
       <c r="F167" s="74"/>
       <c r="G167" s="37"/>
@@ -8076,7 +8086,7 @@
       <c r="A168" s="20"/>
       <c r="B168" s="28"/>
       <c r="C168" s="13"/>
-      <c r="D168" s="240"/>
+      <c r="D168" s="257"/>
       <c r="E168" s="67"/>
       <c r="F168" s="37"/>
       <c r="G168" s="37"/>
@@ -8107,7 +8117,7 @@
       <c r="A169" s="20"/>
       <c r="B169" s="28"/>
       <c r="C169" s="13"/>
-      <c r="D169" s="240"/>
+      <c r="D169" s="257"/>
       <c r="E169" s="67"/>
       <c r="F169" s="37"/>
       <c r="G169" s="37"/>
@@ -8138,7 +8148,7 @@
       <c r="A170" s="20"/>
       <c r="B170" s="28"/>
       <c r="C170" s="28"/>
-      <c r="D170" s="241"/>
+      <c r="D170" s="253"/>
       <c r="E170" s="67"/>
       <c r="F170" s="37"/>
       <c r="G170" s="37"/>
@@ -9478,8 +9488,8 @@
       <c r="H213" s="16"/>
       <c r="I213" s="38"/>
       <c r="J213" s="38"/>
-      <c r="K213" s="249"/>
-      <c r="L213" s="242"/>
+      <c r="K213" s="252"/>
+      <c r="L213" s="259"/>
       <c r="M213" s="18"/>
       <c r="N213" s="4"/>
       <c r="O213" s="4"/>
@@ -9509,8 +9519,8 @@
       <c r="H214" s="16"/>
       <c r="I214" s="71"/>
       <c r="J214" s="71"/>
-      <c r="K214" s="240"/>
-      <c r="L214" s="240"/>
+      <c r="K214" s="257"/>
+      <c r="L214" s="257"/>
       <c r="M214" s="18"/>
       <c r="N214" s="4"/>
       <c r="O214" s="4"/>
@@ -9540,8 +9550,8 @@
       <c r="H215" s="16"/>
       <c r="I215" s="54"/>
       <c r="J215" s="54"/>
-      <c r="K215" s="241"/>
-      <c r="L215" s="241"/>
+      <c r="K215" s="253"/>
+      <c r="L215" s="253"/>
       <c r="M215" s="18"/>
       <c r="N215" s="4"/>
       <c r="O215" s="4"/>
@@ -9749,10 +9759,10 @@
     <row r="222" spans="1:29" ht="15.75" customHeight="1">
       <c r="A222" s="20"/>
       <c r="B222" s="21"/>
-      <c r="C222" s="242"/>
+      <c r="C222" s="259"/>
       <c r="D222" s="13"/>
       <c r="E222" s="16"/>
-      <c r="F222" s="246"/>
+      <c r="F222" s="256"/>
       <c r="G222" s="16"/>
       <c r="H222" s="16"/>
       <c r="I222" s="16"/>
@@ -9780,10 +9790,10 @@
     <row r="223" spans="1:29" ht="15.75" customHeight="1">
       <c r="A223" s="20"/>
       <c r="B223" s="21"/>
-      <c r="C223" s="240"/>
+      <c r="C223" s="257"/>
       <c r="D223" s="13"/>
       <c r="E223" s="16"/>
-      <c r="F223" s="240"/>
+      <c r="F223" s="257"/>
       <c r="G223" s="16"/>
       <c r="H223" s="16"/>
       <c r="I223" s="16"/>
@@ -9811,10 +9821,10 @@
     <row r="224" spans="1:29" ht="15.75" customHeight="1">
       <c r="A224" s="20"/>
       <c r="B224" s="21"/>
-      <c r="C224" s="240"/>
+      <c r="C224" s="257"/>
       <c r="D224" s="13"/>
       <c r="E224" s="16"/>
-      <c r="F224" s="241"/>
+      <c r="F224" s="253"/>
       <c r="G224" s="16"/>
       <c r="H224" s="16"/>
       <c r="I224" s="16"/>
@@ -9842,7 +9852,7 @@
     <row r="225" spans="1:29" ht="15.75" customHeight="1">
       <c r="A225" s="20"/>
       <c r="B225" s="21"/>
-      <c r="C225" s="240"/>
+      <c r="C225" s="257"/>
       <c r="D225" s="13"/>
       <c r="E225" s="16"/>
       <c r="F225" s="16"/>
@@ -9873,7 +9883,7 @@
     <row r="226" spans="1:29" ht="15.75" customHeight="1">
       <c r="A226" s="20"/>
       <c r="B226" s="21"/>
-      <c r="C226" s="240"/>
+      <c r="C226" s="257"/>
       <c r="D226" s="13"/>
       <c r="E226" s="16"/>
       <c r="F226" s="16"/>
@@ -9904,7 +9914,7 @@
     <row r="227" spans="1:29" ht="15.75" customHeight="1">
       <c r="A227" s="20"/>
       <c r="B227" s="21"/>
-      <c r="C227" s="240"/>
+      <c r="C227" s="257"/>
       <c r="D227" s="13"/>
       <c r="E227" s="16"/>
       <c r="F227" s="16"/>
@@ -9935,7 +9945,7 @@
     <row r="228" spans="1:29" ht="15.75" customHeight="1">
       <c r="A228" s="20"/>
       <c r="B228" s="21"/>
-      <c r="C228" s="241"/>
+      <c r="C228" s="253"/>
       <c r="D228" s="13"/>
       <c r="E228" s="16"/>
       <c r="F228" s="16"/>
@@ -9966,7 +9976,7 @@
     <row r="229" spans="1:29" ht="15.75" customHeight="1">
       <c r="A229" s="20"/>
       <c r="B229" s="21"/>
-      <c r="C229" s="244"/>
+      <c r="C229" s="267"/>
       <c r="D229" s="114"/>
       <c r="E229" s="23"/>
       <c r="F229" s="16"/>
@@ -9997,7 +10007,7 @@
     <row r="230" spans="1:29" ht="15.75" customHeight="1">
       <c r="A230" s="20"/>
       <c r="B230" s="21"/>
-      <c r="C230" s="241"/>
+      <c r="C230" s="253"/>
       <c r="D230" s="110"/>
       <c r="E230" s="48"/>
       <c r="F230" s="16"/>
@@ -10059,7 +10069,7 @@
     <row r="232" spans="1:29" ht="30" customHeight="1">
       <c r="A232" s="20"/>
       <c r="B232" s="21"/>
-      <c r="C232" s="244"/>
+      <c r="C232" s="267"/>
       <c r="D232" s="114"/>
       <c r="E232" s="23"/>
       <c r="F232" s="16"/>
@@ -10090,7 +10100,7 @@
     <row r="233" spans="1:29" ht="15.75" customHeight="1">
       <c r="A233" s="20"/>
       <c r="B233" s="21"/>
-      <c r="C233" s="240"/>
+      <c r="C233" s="257"/>
       <c r="D233" s="73"/>
       <c r="E233" s="45"/>
       <c r="F233" s="16"/>
@@ -10121,7 +10131,7 @@
     <row r="234" spans="1:29" ht="15.75" customHeight="1">
       <c r="A234" s="20"/>
       <c r="B234" s="21"/>
-      <c r="C234" s="240"/>
+      <c r="C234" s="257"/>
       <c r="D234" s="73"/>
       <c r="E234" s="45"/>
       <c r="F234" s="16"/>
@@ -10152,7 +10162,7 @@
     <row r="235" spans="1:29" ht="15.75" customHeight="1">
       <c r="A235" s="20"/>
       <c r="B235" s="21"/>
-      <c r="C235" s="240"/>
+      <c r="C235" s="257"/>
       <c r="D235" s="73"/>
       <c r="E235" s="45"/>
       <c r="F235" s="16"/>
@@ -10183,7 +10193,7 @@
     <row r="236" spans="1:29" ht="15.75" customHeight="1">
       <c r="A236" s="20"/>
       <c r="B236" s="21"/>
-      <c r="C236" s="241"/>
+      <c r="C236" s="253"/>
       <c r="D236" s="73"/>
       <c r="E236" s="138"/>
       <c r="F236" s="139"/>
@@ -10563,7 +10573,7 @@
       <c r="H248" s="129"/>
       <c r="I248" s="129"/>
       <c r="J248" s="129"/>
-      <c r="K248" s="257"/>
+      <c r="K248" s="260"/>
       <c r="L248" s="28"/>
       <c r="M248" s="94"/>
       <c r="N248" s="4"/>
@@ -10594,7 +10604,7 @@
       <c r="H249" s="129"/>
       <c r="I249" s="129"/>
       <c r="J249" s="129"/>
-      <c r="K249" s="241"/>
+      <c r="K249" s="253"/>
       <c r="L249" s="28"/>
       <c r="M249" s="94"/>
       <c r="N249" s="4"/>
@@ -10679,7 +10689,7 @@
     <row r="252" spans="1:29" ht="15.75" customHeight="1">
       <c r="A252" s="20"/>
       <c r="B252" s="21"/>
-      <c r="C252" s="244"/>
+      <c r="C252" s="267"/>
       <c r="D252" s="114"/>
       <c r="E252" s="23"/>
       <c r="F252" s="16"/>
@@ -10687,7 +10697,7 @@
       <c r="H252" s="129"/>
       <c r="I252" s="129"/>
       <c r="J252" s="129"/>
-      <c r="K252" s="249"/>
+      <c r="K252" s="252"/>
       <c r="L252" s="28"/>
       <c r="M252" s="94"/>
       <c r="N252" s="4"/>
@@ -10710,7 +10720,7 @@
     <row r="253" spans="1:29" ht="15.75" customHeight="1">
       <c r="A253" s="20"/>
       <c r="B253" s="21"/>
-      <c r="C253" s="241"/>
+      <c r="C253" s="253"/>
       <c r="D253" s="110"/>
       <c r="E253" s="48"/>
       <c r="F253" s="16"/>
@@ -10718,7 +10728,7 @@
       <c r="H253" s="129"/>
       <c r="I253" s="129"/>
       <c r="J253" s="129"/>
-      <c r="K253" s="241"/>
+      <c r="K253" s="253"/>
       <c r="L253" s="28"/>
       <c r="M253" s="94"/>
       <c r="N253" s="4"/>
@@ -10741,7 +10751,7 @@
     <row r="254" spans="1:29" ht="15.75" customHeight="1">
       <c r="A254" s="20"/>
       <c r="B254" s="21"/>
-      <c r="C254" s="242"/>
+      <c r="C254" s="259"/>
       <c r="D254" s="19"/>
       <c r="E254" s="114"/>
       <c r="F254" s="74"/>
@@ -10772,7 +10782,7 @@
     <row r="255" spans="1:29" ht="15.75" customHeight="1">
       <c r="A255" s="20"/>
       <c r="B255" s="21"/>
-      <c r="C255" s="241"/>
+      <c r="C255" s="253"/>
       <c r="D255" s="92"/>
       <c r="E255" s="110"/>
       <c r="F255" s="74"/>
@@ -10834,7 +10844,7 @@
     <row r="257" spans="1:29" ht="15.75" customHeight="1">
       <c r="A257" s="20"/>
       <c r="B257" s="21"/>
-      <c r="C257" s="244"/>
+      <c r="C257" s="267"/>
       <c r="D257" s="114"/>
       <c r="E257" s="114"/>
       <c r="F257" s="74"/>
@@ -10865,7 +10875,7 @@
     <row r="258" spans="1:29" ht="15.75" customHeight="1">
       <c r="A258" s="20"/>
       <c r="B258" s="21"/>
-      <c r="C258" s="240"/>
+      <c r="C258" s="257"/>
       <c r="D258" s="73"/>
       <c r="E258" s="73"/>
       <c r="F258" s="74"/>
@@ -10896,7 +10906,7 @@
     <row r="259" spans="1:29" ht="15.75" customHeight="1">
       <c r="A259" s="20"/>
       <c r="B259" s="21"/>
-      <c r="C259" s="241"/>
+      <c r="C259" s="253"/>
       <c r="D259" s="110"/>
       <c r="E259" s="110"/>
       <c r="F259" s="74"/>
@@ -11081,11 +11091,11 @@
     </row>
     <row r="265" spans="1:29" ht="15.75" customHeight="1">
       <c r="A265" s="25"/>
-      <c r="B265" s="239"/>
-      <c r="C265" s="242"/>
+      <c r="B265" s="277"/>
+      <c r="C265" s="259"/>
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
-      <c r="F265" s="242"/>
+      <c r="F265" s="259"/>
       <c r="G265" s="149"/>
       <c r="H265" s="149"/>
       <c r="I265" s="149"/>
@@ -11112,11 +11122,11 @@
     </row>
     <row r="266" spans="1:29" ht="15.75" customHeight="1">
       <c r="A266" s="25"/>
-      <c r="B266" s="240"/>
-      <c r="C266" s="240"/>
+      <c r="B266" s="257"/>
+      <c r="C266" s="257"/>
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
-      <c r="F266" s="240"/>
+      <c r="F266" s="257"/>
       <c r="G266" s="149"/>
       <c r="H266" s="149"/>
       <c r="I266" s="149"/>
@@ -11143,11 +11153,11 @@
     </row>
     <row r="267" spans="1:29" ht="15.75" customHeight="1">
       <c r="A267" s="25"/>
-      <c r="B267" s="240"/>
-      <c r="C267" s="240"/>
+      <c r="B267" s="257"/>
+      <c r="C267" s="257"/>
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
-      <c r="F267" s="240"/>
+      <c r="F267" s="257"/>
       <c r="G267" s="149"/>
       <c r="H267" s="149"/>
       <c r="I267" s="149"/>
@@ -11174,11 +11184,11 @@
     </row>
     <row r="268" spans="1:29" ht="15.75" customHeight="1">
       <c r="A268" s="25"/>
-      <c r="B268" s="240"/>
-      <c r="C268" s="240"/>
+      <c r="B268" s="257"/>
+      <c r="C268" s="257"/>
       <c r="D268" s="13"/>
       <c r="E268" s="13"/>
-      <c r="F268" s="240"/>
+      <c r="F268" s="257"/>
       <c r="G268" s="149"/>
       <c r="H268" s="149"/>
       <c r="I268" s="149"/>
@@ -11205,11 +11215,11 @@
     </row>
     <row r="269" spans="1:29" ht="15.75" customHeight="1">
       <c r="A269" s="25"/>
-      <c r="B269" s="240"/>
-      <c r="C269" s="240"/>
+      <c r="B269" s="257"/>
+      <c r="C269" s="257"/>
       <c r="D269" s="13"/>
       <c r="E269" s="13"/>
-      <c r="F269" s="240"/>
+      <c r="F269" s="257"/>
       <c r="G269" s="149"/>
       <c r="H269" s="149"/>
       <c r="I269" s="149"/>
@@ -11236,11 +11246,11 @@
     </row>
     <row r="270" spans="1:29" ht="15.75" customHeight="1">
       <c r="A270" s="25"/>
-      <c r="B270" s="240"/>
-      <c r="C270" s="240"/>
+      <c r="B270" s="257"/>
+      <c r="C270" s="257"/>
       <c r="D270" s="13"/>
       <c r="E270" s="13"/>
-      <c r="F270" s="240"/>
+      <c r="F270" s="257"/>
       <c r="G270" s="150"/>
       <c r="H270" s="150"/>
       <c r="I270" s="150"/>
@@ -11267,11 +11277,11 @@
     </row>
     <row r="271" spans="1:29" ht="15.75" customHeight="1">
       <c r="A271" s="25"/>
-      <c r="B271" s="240"/>
-      <c r="C271" s="240"/>
+      <c r="B271" s="257"/>
+      <c r="C271" s="257"/>
       <c r="D271" s="13"/>
       <c r="E271" s="13"/>
-      <c r="F271" s="240"/>
+      <c r="F271" s="257"/>
       <c r="G271" s="149"/>
       <c r="H271" s="149"/>
       <c r="I271" s="149"/>
@@ -11298,11 +11308,11 @@
     </row>
     <row r="272" spans="1:29" ht="15.75" customHeight="1">
       <c r="A272" s="25"/>
-      <c r="B272" s="240"/>
-      <c r="C272" s="240"/>
+      <c r="B272" s="257"/>
+      <c r="C272" s="257"/>
       <c r="D272" s="13"/>
       <c r="E272" s="13"/>
-      <c r="F272" s="241"/>
+      <c r="F272" s="253"/>
       <c r="G272" s="149"/>
       <c r="H272" s="149"/>
       <c r="I272" s="149"/>
@@ -11329,8 +11339,8 @@
     </row>
     <row r="273" spans="1:29" ht="15.75" customHeight="1">
       <c r="A273" s="25"/>
-      <c r="B273" s="240"/>
-      <c r="C273" s="240"/>
+      <c r="B273" s="257"/>
+      <c r="C273" s="257"/>
       <c r="D273" s="13"/>
       <c r="E273" s="28"/>
       <c r="F273" s="28"/>
@@ -11360,8 +11370,8 @@
     </row>
     <row r="274" spans="1:29" ht="15.75" customHeight="1">
       <c r="A274" s="25"/>
-      <c r="B274" s="240"/>
-      <c r="C274" s="240"/>
+      <c r="B274" s="257"/>
+      <c r="C274" s="257"/>
       <c r="D274" s="13"/>
       <c r="E274" s="28"/>
       <c r="F274" s="28"/>
@@ -11391,11 +11401,11 @@
     </row>
     <row r="275" spans="1:29" ht="15.75" customHeight="1">
       <c r="A275" s="25"/>
-      <c r="B275" s="240"/>
-      <c r="C275" s="240"/>
+      <c r="B275" s="257"/>
+      <c r="C275" s="257"/>
       <c r="D275" s="19"/>
       <c r="E275" s="19"/>
-      <c r="F275" s="242"/>
+      <c r="F275" s="259"/>
       <c r="G275" s="30"/>
       <c r="H275" s="30"/>
       <c r="I275" s="30"/>
@@ -11422,11 +11432,11 @@
     </row>
     <row r="276" spans="1:29" ht="15.75" customHeight="1">
       <c r="A276" s="25"/>
-      <c r="B276" s="240"/>
-      <c r="C276" s="240"/>
+      <c r="B276" s="257"/>
+      <c r="C276" s="257"/>
       <c r="D276" s="108"/>
       <c r="E276" s="108"/>
-      <c r="F276" s="240"/>
+      <c r="F276" s="257"/>
       <c r="G276" s="25"/>
       <c r="H276" s="25"/>
       <c r="I276" s="25"/>
@@ -11453,11 +11463,11 @@
     </row>
     <row r="277" spans="1:29" ht="15.75" customHeight="1">
       <c r="A277" s="25"/>
-      <c r="B277" s="240"/>
-      <c r="C277" s="240"/>
+      <c r="B277" s="257"/>
+      <c r="C277" s="257"/>
       <c r="D277" s="108"/>
       <c r="E277" s="108"/>
-      <c r="F277" s="240"/>
+      <c r="F277" s="257"/>
       <c r="G277" s="25"/>
       <c r="H277" s="25"/>
       <c r="I277" s="25"/>
@@ -11484,11 +11494,11 @@
     </row>
     <row r="278" spans="1:29" ht="15.75" customHeight="1">
       <c r="A278" s="25"/>
-      <c r="B278" s="240"/>
-      <c r="C278" s="241"/>
+      <c r="B278" s="257"/>
+      <c r="C278" s="253"/>
       <c r="D278" s="92"/>
       <c r="E278" s="92"/>
-      <c r="F278" s="241"/>
+      <c r="F278" s="253"/>
       <c r="G278" s="25"/>
       <c r="H278" s="25"/>
       <c r="I278" s="25"/>
@@ -11515,7 +11525,7 @@
     </row>
     <row r="279" spans="1:29" ht="15.75" customHeight="1">
       <c r="A279" s="25"/>
-      <c r="B279" s="240"/>
+      <c r="B279" s="257"/>
       <c r="C279" s="13"/>
       <c r="D279" s="108"/>
       <c r="E279" s="108"/>
@@ -11546,11 +11556,11 @@
     </row>
     <row r="280" spans="1:29" ht="15.75" customHeight="1">
       <c r="A280" s="25"/>
-      <c r="B280" s="240"/>
-      <c r="C280" s="242"/>
+      <c r="B280" s="257"/>
+      <c r="C280" s="259"/>
       <c r="D280" s="19"/>
       <c r="E280" s="99"/>
-      <c r="F280" s="243"/>
+      <c r="F280" s="278"/>
       <c r="G280" s="37"/>
       <c r="H280" s="37"/>
       <c r="I280" s="37"/>
@@ -11577,11 +11587,11 @@
     </row>
     <row r="281" spans="1:29" ht="15.75" customHeight="1">
       <c r="A281" s="25"/>
-      <c r="B281" s="240"/>
-      <c r="C281" s="240"/>
+      <c r="B281" s="257"/>
+      <c r="C281" s="257"/>
       <c r="D281" s="92"/>
       <c r="E281" s="113"/>
-      <c r="F281" s="241"/>
+      <c r="F281" s="253"/>
       <c r="G281" s="37"/>
       <c r="H281" s="37"/>
       <c r="I281" s="37"/>
@@ -11608,11 +11618,11 @@
     </row>
     <row r="282" spans="1:29" ht="15.75" customHeight="1">
       <c r="A282" s="25"/>
-      <c r="B282" s="240"/>
-      <c r="C282" s="240"/>
+      <c r="B282" s="257"/>
+      <c r="C282" s="257"/>
       <c r="D282" s="13"/>
       <c r="E282" s="20"/>
-      <c r="F282" s="243"/>
+      <c r="F282" s="278"/>
       <c r="G282" s="37"/>
       <c r="H282" s="37"/>
       <c r="I282" s="37"/>
@@ -11639,11 +11649,11 @@
     </row>
     <row r="283" spans="1:29" ht="15.75" customHeight="1">
       <c r="A283" s="25"/>
-      <c r="B283" s="240"/>
-      <c r="C283" s="241"/>
+      <c r="B283" s="257"/>
+      <c r="C283" s="253"/>
       <c r="D283" s="13"/>
       <c r="E283" s="20"/>
-      <c r="F283" s="241"/>
+      <c r="F283" s="253"/>
       <c r="G283" s="37"/>
       <c r="H283" s="37"/>
       <c r="I283" s="37"/>
@@ -11670,7 +11680,7 @@
     </row>
     <row r="284" spans="1:29" ht="15.75" customHeight="1">
       <c r="A284" s="25"/>
-      <c r="B284" s="240"/>
+      <c r="B284" s="257"/>
       <c r="C284" s="28"/>
       <c r="D284" s="28"/>
       <c r="E284" s="25"/>
@@ -11701,11 +11711,11 @@
     </row>
     <row r="285" spans="1:29" ht="15.75" customHeight="1">
       <c r="A285" s="25"/>
-      <c r="B285" s="240"/>
-      <c r="C285" s="242"/>
+      <c r="B285" s="257"/>
+      <c r="C285" s="259"/>
       <c r="D285" s="19"/>
       <c r="E285" s="19"/>
-      <c r="F285" s="242"/>
+      <c r="F285" s="259"/>
       <c r="G285" s="30"/>
       <c r="H285" s="30"/>
       <c r="I285" s="30"/>
@@ -11732,11 +11742,11 @@
     </row>
     <row r="286" spans="1:29" ht="15.75" customHeight="1">
       <c r="A286" s="25"/>
-      <c r="B286" s="240"/>
-      <c r="C286" s="240"/>
+      <c r="B286" s="257"/>
+      <c r="C286" s="257"/>
       <c r="D286" s="108"/>
       <c r="E286" s="108"/>
-      <c r="F286" s="240"/>
+      <c r="F286" s="257"/>
       <c r="G286" s="30"/>
       <c r="H286" s="30"/>
       <c r="I286" s="30"/>
@@ -11763,11 +11773,11 @@
     </row>
     <row r="287" spans="1:29" ht="15.75" customHeight="1">
       <c r="A287" s="25"/>
-      <c r="B287" s="240"/>
-      <c r="C287" s="240"/>
+      <c r="B287" s="257"/>
+      <c r="C287" s="257"/>
       <c r="D287" s="108"/>
       <c r="E287" s="108"/>
-      <c r="F287" s="240"/>
+      <c r="F287" s="257"/>
       <c r="G287" s="30"/>
       <c r="H287" s="30"/>
       <c r="I287" s="30"/>
@@ -11794,11 +11804,11 @@
     </row>
     <row r="288" spans="1:29" ht="15.75" customHeight="1">
       <c r="A288" s="25"/>
-      <c r="B288" s="240"/>
-      <c r="C288" s="240"/>
+      <c r="B288" s="257"/>
+      <c r="C288" s="257"/>
       <c r="D288" s="108"/>
       <c r="E288" s="108"/>
-      <c r="F288" s="240"/>
+      <c r="F288" s="257"/>
       <c r="G288" s="30"/>
       <c r="H288" s="30"/>
       <c r="I288" s="30"/>
@@ -11825,11 +11835,11 @@
     </row>
     <row r="289" spans="1:29" ht="15.75" customHeight="1">
       <c r="A289" s="25"/>
-      <c r="B289" s="240"/>
-      <c r="C289" s="240"/>
+      <c r="B289" s="257"/>
+      <c r="C289" s="257"/>
       <c r="D289" s="108"/>
       <c r="E289" s="108"/>
-      <c r="F289" s="240"/>
+      <c r="F289" s="257"/>
       <c r="G289" s="149"/>
       <c r="H289" s="149"/>
       <c r="I289" s="149"/>
@@ -11856,11 +11866,11 @@
     </row>
     <row r="290" spans="1:29" ht="15.75" customHeight="1">
       <c r="A290" s="25"/>
-      <c r="B290" s="240"/>
-      <c r="C290" s="240"/>
+      <c r="B290" s="257"/>
+      <c r="C290" s="257"/>
       <c r="D290" s="92"/>
       <c r="E290" s="92"/>
-      <c r="F290" s="241"/>
+      <c r="F290" s="253"/>
       <c r="G290" s="149"/>
       <c r="H290" s="149"/>
       <c r="I290" s="149"/>
@@ -11887,11 +11897,11 @@
     </row>
     <row r="291" spans="1:29" ht="15.75" customHeight="1">
       <c r="A291" s="25"/>
-      <c r="B291" s="240"/>
-      <c r="C291" s="240"/>
+      <c r="B291" s="257"/>
+      <c r="C291" s="257"/>
       <c r="D291" s="19"/>
       <c r="E291" s="19"/>
-      <c r="F291" s="242"/>
+      <c r="F291" s="259"/>
       <c r="G291" s="30"/>
       <c r="H291" s="30"/>
       <c r="I291" s="30"/>
@@ -11918,11 +11928,11 @@
     </row>
     <row r="292" spans="1:29" ht="15.75" customHeight="1">
       <c r="A292" s="25"/>
-      <c r="B292" s="240"/>
-      <c r="C292" s="240"/>
+      <c r="B292" s="257"/>
+      <c r="C292" s="257"/>
       <c r="D292" s="108"/>
       <c r="E292" s="108"/>
-      <c r="F292" s="240"/>
+      <c r="F292" s="257"/>
       <c r="G292" s="25"/>
       <c r="H292" s="25"/>
       <c r="I292" s="25"/>
@@ -11949,11 +11959,11 @@
     </row>
     <row r="293" spans="1:29" ht="15.75" customHeight="1">
       <c r="A293" s="25"/>
-      <c r="B293" s="240"/>
-      <c r="C293" s="240"/>
+      <c r="B293" s="257"/>
+      <c r="C293" s="257"/>
       <c r="D293" s="108"/>
       <c r="E293" s="108"/>
-      <c r="F293" s="240"/>
+      <c r="F293" s="257"/>
       <c r="G293" s="25"/>
       <c r="H293" s="25"/>
       <c r="I293" s="25"/>
@@ -11980,11 +11990,11 @@
     </row>
     <row r="294" spans="1:29" ht="15.75" customHeight="1">
       <c r="A294" s="25"/>
-      <c r="B294" s="241"/>
-      <c r="C294" s="241"/>
+      <c r="B294" s="253"/>
+      <c r="C294" s="253"/>
       <c r="D294" s="92"/>
       <c r="E294" s="92"/>
-      <c r="F294" s="241"/>
+      <c r="F294" s="253"/>
       <c r="G294" s="25"/>
       <c r="H294" s="25"/>
       <c r="I294" s="25"/>
@@ -14760,11 +14770,79 @@
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C11:C17"/>
-    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="K32:K38"/>
+    <mergeCell ref="L32:L38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="D32:D44"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="F39:F44"/>
+    <mergeCell ref="G39:G44"/>
+    <mergeCell ref="H39:H44"/>
+    <mergeCell ref="I39:I44"/>
+    <mergeCell ref="J39:J44"/>
+    <mergeCell ref="K39:K44"/>
+    <mergeCell ref="L39:L44"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="D18:D31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="C254:C255"/>
+    <mergeCell ref="C280:C283"/>
+    <mergeCell ref="C285:C294"/>
+    <mergeCell ref="F285:F290"/>
+    <mergeCell ref="F291:F294"/>
+    <mergeCell ref="C257:C259"/>
+    <mergeCell ref="B265:B294"/>
+    <mergeCell ref="C265:C278"/>
+    <mergeCell ref="F265:F272"/>
+    <mergeCell ref="F275:F278"/>
+    <mergeCell ref="F280:F281"/>
+    <mergeCell ref="F282:F283"/>
+    <mergeCell ref="C252:C253"/>
+    <mergeCell ref="D97:D103"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="D51:D60"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="D71:D81"/>
+    <mergeCell ref="D83:D92"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D150:D160"/>
+    <mergeCell ref="D162:D170"/>
+    <mergeCell ref="C222:C228"/>
+    <mergeCell ref="C229:C230"/>
+    <mergeCell ref="C232:C236"/>
+    <mergeCell ref="K252:K253"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F222:F224"/>
+    <mergeCell ref="M150:M157"/>
+    <mergeCell ref="K213:K215"/>
+    <mergeCell ref="L213:L215"/>
+    <mergeCell ref="K248:K249"/>
+    <mergeCell ref="F11:F17"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="K19:K24"/>
+    <mergeCell ref="L19:L24"/>
+    <mergeCell ref="H25:H31"/>
+    <mergeCell ref="I25:I31"/>
+    <mergeCell ref="G19:G24"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L11:L17"/>
@@ -14781,80 +14859,12 @@
     <mergeCell ref="I32:I38"/>
     <mergeCell ref="J32:J38"/>
     <mergeCell ref="E11:E17"/>
-    <mergeCell ref="K252:K253"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F222:F224"/>
-    <mergeCell ref="M150:M157"/>
-    <mergeCell ref="K213:K215"/>
-    <mergeCell ref="L213:L215"/>
-    <mergeCell ref="K248:K249"/>
-    <mergeCell ref="F11:F17"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="J19:J24"/>
-    <mergeCell ref="K19:K24"/>
-    <mergeCell ref="L19:L24"/>
-    <mergeCell ref="H25:H31"/>
-    <mergeCell ref="I25:I31"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="D97:D103"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="D51:D60"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="D71:D81"/>
-    <mergeCell ref="D83:D92"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D150:D160"/>
-    <mergeCell ref="D162:D170"/>
-    <mergeCell ref="G19:G24"/>
-    <mergeCell ref="B265:B294"/>
-    <mergeCell ref="C265:C278"/>
-    <mergeCell ref="F265:F272"/>
-    <mergeCell ref="F275:F278"/>
-    <mergeCell ref="F280:F281"/>
-    <mergeCell ref="F282:F283"/>
-    <mergeCell ref="C254:C255"/>
-    <mergeCell ref="C280:C283"/>
-    <mergeCell ref="C285:C294"/>
-    <mergeCell ref="F285:F290"/>
-    <mergeCell ref="F291:F294"/>
-    <mergeCell ref="C257:C259"/>
-    <mergeCell ref="C222:C228"/>
-    <mergeCell ref="C229:C230"/>
-    <mergeCell ref="C232:C236"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="A45:A50"/>
     <mergeCell ref="A32:A38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="D18:D31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="F25:F31"/>
-    <mergeCell ref="G25:G31"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="F19:F24"/>
-    <mergeCell ref="K32:K38"/>
-    <mergeCell ref="L32:L38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="D32:D44"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="F39:F44"/>
-    <mergeCell ref="G39:G44"/>
-    <mergeCell ref="H39:H44"/>
-    <mergeCell ref="I39:I44"/>
-    <mergeCell ref="J39:J44"/>
-    <mergeCell ref="K39:K44"/>
-    <mergeCell ref="L39:L44"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="C39:C44"/>
   </mergeCells>
   <conditionalFormatting sqref="K196:K201 K203:K204 K241 K255:K264 L97:L103 L11 L39:L46 L48:L49 L51:L69 L71:L81 L83:L86 L88:L92 L94:L95 L105:L362 L18:L19 L25:L32">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -14881,9 +14891,13 @@
       <formula1>"Passed,Failed,Not Executed,Out of Scope"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J19:J24" r:id="rId1" display="Click Here"/>
+    <hyperlink ref="J25:J31" r:id="rId2" display="Click Here"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -14914,39 +14928,39 @@
     <row r="2" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="3" spans="1:26" ht="8.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="25.5" customHeight="1">
-      <c r="B4" s="314" t="s">
+      <c r="B4" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="315"/>
-      <c r="F4" s="315"/>
-      <c r="G4" s="316"/>
+      <c r="C4" s="287"/>
+      <c r="D4" s="287"/>
+      <c r="E4" s="287"/>
+      <c r="F4" s="287"/>
+      <c r="G4" s="288"/>
       <c r="K4" s="156"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="B5" s="157" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="301" t="s">
+      <c r="C5" s="289" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
-      <c r="G5" s="303"/>
+      <c r="D5" s="290"/>
+      <c r="E5" s="290"/>
+      <c r="F5" s="290"/>
+      <c r="G5" s="291"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="B6" s="158" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="301" t="s">
+      <c r="C6" s="289" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="302"/>
-      <c r="E6" s="302"/>
-      <c r="F6" s="302"/>
-      <c r="G6" s="303"/>
+      <c r="D6" s="290"/>
+      <c r="E6" s="290"/>
+      <c r="F6" s="290"/>
+      <c r="G6" s="291"/>
       <c r="I6" s="159" t="s">
         <v>26</v>
       </c>
@@ -14961,13 +14975,13 @@
       <c r="B7" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="301" t="s">
+      <c r="C7" s="289" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="302"/>
-      <c r="E7" s="302"/>
-      <c r="F7" s="302"/>
-      <c r="G7" s="303"/>
+      <c r="D7" s="290"/>
+      <c r="E7" s="290"/>
+      <c r="F7" s="290"/>
+      <c r="G7" s="291"/>
       <c r="I7" s="161">
         <f>C15</f>
         <v>4</v>
@@ -14982,13 +14996,13 @@
       <c r="B8" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="301" t="s">
+      <c r="C8" s="289" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="302"/>
-      <c r="E8" s="302"/>
-      <c r="F8" s="302"/>
-      <c r="G8" s="303"/>
+      <c r="D8" s="290"/>
+      <c r="E8" s="290"/>
+      <c r="F8" s="290"/>
+      <c r="G8" s="291"/>
       <c r="I8" s="161">
         <f>D15</f>
         <v>2</v>
@@ -15003,13 +15017,13 @@
       <c r="B9" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="301" t="s">
+      <c r="C9" s="289" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="302"/>
-      <c r="E9" s="302"/>
-      <c r="F9" s="302"/>
-      <c r="G9" s="303"/>
+      <c r="D9" s="290"/>
+      <c r="E9" s="290"/>
+      <c r="F9" s="290"/>
+      <c r="G9" s="291"/>
       <c r="I9" s="161">
         <f>E15</f>
         <v>0</v>
@@ -15033,13 +15047,13 @@
       <c r="B10" s="157" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="301" t="s">
+      <c r="C10" s="289" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="302"/>
-      <c r="E10" s="302"/>
-      <c r="F10" s="302"/>
-      <c r="G10" s="303"/>
+      <c r="D10" s="290"/>
+      <c r="E10" s="290"/>
+      <c r="F10" s="290"/>
+      <c r="G10" s="291"/>
       <c r="I10" s="161">
         <f>F15</f>
         <v>0</v>
@@ -15058,22 +15072,22 @@
       <c r="P10" s="78"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B11" s="304" t="s">
+      <c r="B11" s="300" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="305"/>
-      <c r="D11" s="305"/>
-      <c r="E11" s="305"/>
-      <c r="F11" s="305"/>
-      <c r="G11" s="306"/>
+      <c r="C11" s="301"/>
+      <c r="D11" s="301"/>
+      <c r="E11" s="301"/>
+      <c r="F11" s="301"/>
+      <c r="G11" s="302"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B12" s="298"/>
-      <c r="C12" s="299"/>
-      <c r="D12" s="299"/>
-      <c r="E12" s="299"/>
-      <c r="F12" s="299"/>
-      <c r="G12" s="300"/>
+      <c r="B12" s="297"/>
+      <c r="C12" s="298"/>
+      <c r="D12" s="298"/>
+      <c r="E12" s="298"/>
+      <c r="F12" s="298"/>
+      <c r="G12" s="299"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="B13" s="167" t="s">
@@ -15208,20 +15222,20 @@
       <c r="R17" s="170"/>
     </row>
     <row r="18" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B18" s="307" t="s">
+      <c r="B18" s="303" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="308"/>
-      <c r="D18" s="308"/>
-      <c r="E18" s="308"/>
-      <c r="F18" s="308"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="304"/>
+      <c r="E18" s="304"/>
+      <c r="F18" s="304"/>
       <c r="G18" s="255"/>
     </row>
     <row r="19" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B19" s="309" t="s">
+      <c r="B19" s="305" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="308"/>
+      <c r="C19" s="304"/>
       <c r="D19" s="255"/>
       <c r="E19" s="185"/>
       <c r="F19" s="185" t="s">
@@ -15232,10 +15246,10 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B20" s="310" t="s">
+      <c r="B20" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="308"/>
+      <c r="C20" s="304"/>
       <c r="D20" s="255"/>
       <c r="E20" s="186"/>
       <c r="F20" s="186" t="s">
@@ -15246,10 +15260,10 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B21" s="310" t="s">
+      <c r="B21" s="306" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="308"/>
+      <c r="C21" s="304"/>
       <c r="D21" s="255"/>
       <c r="E21" s="186"/>
       <c r="F21" s="186" t="s">
@@ -15261,306 +15275,306 @@
     </row>
     <row r="22" spans="2:18" ht="15.75" customHeight="1"/>
     <row r="23" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B23" s="313"/>
-      <c r="C23" s="311" t="s">
+      <c r="B23" s="311"/>
+      <c r="C23" s="307" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="312" t="s">
+      <c r="D23" s="310" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="294"/>
-      <c r="F23" s="294"/>
-      <c r="G23" s="295"/>
+      <c r="E23" s="293"/>
+      <c r="F23" s="293"/>
+      <c r="G23" s="294"/>
     </row>
     <row r="24" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B24" s="289"/>
-      <c r="C24" s="289"/>
-      <c r="D24" s="296"/>
-      <c r="E24" s="248"/>
-      <c r="F24" s="248"/>
-      <c r="G24" s="297"/>
+      <c r="B24" s="308"/>
+      <c r="C24" s="308"/>
+      <c r="D24" s="295"/>
+      <c r="E24" s="229"/>
+      <c r="F24" s="229"/>
+      <c r="G24" s="296"/>
     </row>
     <row r="25" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B25" s="289"/>
-      <c r="C25" s="289"/>
-      <c r="D25" s="296"/>
-      <c r="E25" s="248"/>
-      <c r="F25" s="248"/>
-      <c r="G25" s="297"/>
+      <c r="B25" s="308"/>
+      <c r="C25" s="308"/>
+      <c r="D25" s="295"/>
+      <c r="E25" s="229"/>
+      <c r="F25" s="229"/>
+      <c r="G25" s="296"/>
     </row>
     <row r="26" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B26" s="290"/>
-      <c r="C26" s="290"/>
-      <c r="D26" s="298"/>
-      <c r="E26" s="299"/>
-      <c r="F26" s="299"/>
-      <c r="G26" s="300"/>
+      <c r="B26" s="309"/>
+      <c r="C26" s="309"/>
+      <c r="D26" s="297"/>
+      <c r="E26" s="298"/>
+      <c r="F26" s="298"/>
+      <c r="G26" s="299"/>
     </row>
     <row r="27" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B27" s="291" t="s">
+      <c r="B27" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="288" t="s">
+      <c r="C27" s="313" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="293" t="s">
+      <c r="D27" s="292" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="294"/>
-      <c r="F27" s="294"/>
-      <c r="G27" s="295"/>
+      <c r="E27" s="293"/>
+      <c r="F27" s="293"/>
+      <c r="G27" s="294"/>
     </row>
     <row r="28" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B28" s="289"/>
-      <c r="C28" s="289"/>
-      <c r="D28" s="296"/>
-      <c r="E28" s="248"/>
-      <c r="F28" s="248"/>
-      <c r="G28" s="297"/>
+      <c r="B28" s="308"/>
+      <c r="C28" s="308"/>
+      <c r="D28" s="295"/>
+      <c r="E28" s="229"/>
+      <c r="F28" s="229"/>
+      <c r="G28" s="296"/>
     </row>
     <row r="29" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B29" s="289"/>
-      <c r="C29" s="289"/>
-      <c r="D29" s="296"/>
-      <c r="E29" s="248"/>
-      <c r="F29" s="248"/>
-      <c r="G29" s="297"/>
+      <c r="B29" s="308"/>
+      <c r="C29" s="308"/>
+      <c r="D29" s="295"/>
+      <c r="E29" s="229"/>
+      <c r="F29" s="229"/>
+      <c r="G29" s="296"/>
     </row>
     <row r="30" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B30" s="290"/>
-      <c r="C30" s="290"/>
-      <c r="D30" s="298"/>
-      <c r="E30" s="299"/>
-      <c r="F30" s="299"/>
-      <c r="G30" s="300"/>
+      <c r="B30" s="309"/>
+      <c r="C30" s="309"/>
+      <c r="D30" s="297"/>
+      <c r="E30" s="298"/>
+      <c r="F30" s="298"/>
+      <c r="G30" s="299"/>
     </row>
     <row r="31" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B31" s="291" t="s">
+      <c r="B31" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="288" t="s">
+      <c r="C31" s="313" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="293" t="s">
+      <c r="D31" s="292" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="294"/>
-      <c r="F31" s="294"/>
-      <c r="G31" s="295"/>
+      <c r="E31" s="293"/>
+      <c r="F31" s="293"/>
+      <c r="G31" s="294"/>
     </row>
     <row r="32" spans="2:18" ht="15.75" customHeight="1">
-      <c r="B32" s="289"/>
-      <c r="C32" s="289"/>
-      <c r="D32" s="296"/>
-      <c r="E32" s="248"/>
-      <c r="F32" s="248"/>
-      <c r="G32" s="297"/>
+      <c r="B32" s="308"/>
+      <c r="C32" s="308"/>
+      <c r="D32" s="295"/>
+      <c r="E32" s="229"/>
+      <c r="F32" s="229"/>
+      <c r="G32" s="296"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B33" s="289"/>
-      <c r="C33" s="289"/>
-      <c r="D33" s="296"/>
-      <c r="E33" s="248"/>
-      <c r="F33" s="248"/>
-      <c r="G33" s="297"/>
+      <c r="B33" s="308"/>
+      <c r="C33" s="308"/>
+      <c r="D33" s="295"/>
+      <c r="E33" s="229"/>
+      <c r="F33" s="229"/>
+      <c r="G33" s="296"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B34" s="290"/>
-      <c r="C34" s="290"/>
-      <c r="D34" s="298"/>
-      <c r="E34" s="299"/>
-      <c r="F34" s="299"/>
-      <c r="G34" s="300"/>
+      <c r="B34" s="309"/>
+      <c r="C34" s="309"/>
+      <c r="D34" s="297"/>
+      <c r="E34" s="298"/>
+      <c r="F34" s="298"/>
+      <c r="G34" s="299"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B35" s="291" t="s">
+      <c r="B35" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="288" t="s">
+      <c r="C35" s="313" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="293" t="s">
+      <c r="D35" s="292" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="294"/>
-      <c r="F35" s="294"/>
-      <c r="G35" s="295"/>
+      <c r="E35" s="293"/>
+      <c r="F35" s="293"/>
+      <c r="G35" s="294"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B36" s="289"/>
-      <c r="C36" s="289"/>
-      <c r="D36" s="296"/>
-      <c r="E36" s="248"/>
-      <c r="F36" s="248"/>
-      <c r="G36" s="297"/>
+      <c r="B36" s="308"/>
+      <c r="C36" s="308"/>
+      <c r="D36" s="295"/>
+      <c r="E36" s="229"/>
+      <c r="F36" s="229"/>
+      <c r="G36" s="296"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B37" s="289"/>
-      <c r="C37" s="289"/>
-      <c r="D37" s="296"/>
-      <c r="E37" s="248"/>
-      <c r="F37" s="248"/>
-      <c r="G37" s="297"/>
+      <c r="B37" s="308"/>
+      <c r="C37" s="308"/>
+      <c r="D37" s="295"/>
+      <c r="E37" s="229"/>
+      <c r="F37" s="229"/>
+      <c r="G37" s="296"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B38" s="290"/>
-      <c r="C38" s="290"/>
-      <c r="D38" s="298"/>
-      <c r="E38" s="299"/>
-      <c r="F38" s="299"/>
-      <c r="G38" s="300"/>
+      <c r="B38" s="309"/>
+      <c r="C38" s="309"/>
+      <c r="D38" s="297"/>
+      <c r="E38" s="298"/>
+      <c r="F38" s="298"/>
+      <c r="G38" s="299"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B39" s="291" t="s">
+      <c r="B39" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="288" t="s">
+      <c r="C39" s="313" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="293" t="s">
+      <c r="D39" s="292" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="294"/>
-      <c r="F39" s="294"/>
-      <c r="G39" s="295"/>
+      <c r="E39" s="293"/>
+      <c r="F39" s="293"/>
+      <c r="G39" s="294"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B40" s="289"/>
-      <c r="C40" s="289"/>
-      <c r="D40" s="296"/>
-      <c r="E40" s="248"/>
-      <c r="F40" s="248"/>
-      <c r="G40" s="297"/>
+      <c r="B40" s="308"/>
+      <c r="C40" s="308"/>
+      <c r="D40" s="295"/>
+      <c r="E40" s="229"/>
+      <c r="F40" s="229"/>
+      <c r="G40" s="296"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B41" s="289"/>
-      <c r="C41" s="289"/>
-      <c r="D41" s="296"/>
-      <c r="E41" s="248"/>
-      <c r="F41" s="248"/>
-      <c r="G41" s="297"/>
+      <c r="B41" s="308"/>
+      <c r="C41" s="308"/>
+      <c r="D41" s="295"/>
+      <c r="E41" s="229"/>
+      <c r="F41" s="229"/>
+      <c r="G41" s="296"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B42" s="290"/>
-      <c r="C42" s="290"/>
-      <c r="D42" s="298"/>
-      <c r="E42" s="299"/>
-      <c r="F42" s="299"/>
-      <c r="G42" s="300"/>
+      <c r="B42" s="309"/>
+      <c r="C42" s="309"/>
+      <c r="D42" s="297"/>
+      <c r="E42" s="298"/>
+      <c r="F42" s="298"/>
+      <c r="G42" s="299"/>
     </row>
     <row r="43" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B43" s="291" t="s">
+      <c r="B43" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="292" t="s">
+      <c r="C43" s="314" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="293" t="s">
+      <c r="D43" s="292" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="294"/>
-      <c r="F43" s="294"/>
-      <c r="G43" s="295"/>
+      <c r="E43" s="293"/>
+      <c r="F43" s="293"/>
+      <c r="G43" s="294"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B44" s="289"/>
-      <c r="C44" s="289"/>
-      <c r="D44" s="296"/>
-      <c r="E44" s="248"/>
-      <c r="F44" s="248"/>
-      <c r="G44" s="297"/>
+      <c r="B44" s="308"/>
+      <c r="C44" s="308"/>
+      <c r="D44" s="295"/>
+      <c r="E44" s="229"/>
+      <c r="F44" s="229"/>
+      <c r="G44" s="296"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B45" s="289"/>
-      <c r="C45" s="289"/>
-      <c r="D45" s="296"/>
-      <c r="E45" s="248"/>
-      <c r="F45" s="248"/>
-      <c r="G45" s="297"/>
+      <c r="B45" s="308"/>
+      <c r="C45" s="308"/>
+      <c r="D45" s="295"/>
+      <c r="E45" s="229"/>
+      <c r="F45" s="229"/>
+      <c r="G45" s="296"/>
     </row>
     <row r="46" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B46" s="290"/>
-      <c r="C46" s="290"/>
-      <c r="D46" s="298"/>
-      <c r="E46" s="299"/>
-      <c r="F46" s="299"/>
-      <c r="G46" s="300"/>
+      <c r="B46" s="309"/>
+      <c r="C46" s="309"/>
+      <c r="D46" s="297"/>
+      <c r="E46" s="298"/>
+      <c r="F46" s="298"/>
+      <c r="G46" s="299"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B47" s="291" t="s">
+      <c r="B47" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="292" t="s">
+      <c r="C47" s="314" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="293" t="s">
+      <c r="D47" s="292" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="294"/>
-      <c r="F47" s="294"/>
-      <c r="G47" s="295"/>
+      <c r="E47" s="293"/>
+      <c r="F47" s="293"/>
+      <c r="G47" s="294"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B48" s="289"/>
-      <c r="C48" s="289"/>
-      <c r="D48" s="296"/>
-      <c r="E48" s="248"/>
-      <c r="F48" s="248"/>
-      <c r="G48" s="297"/>
+      <c r="B48" s="308"/>
+      <c r="C48" s="308"/>
+      <c r="D48" s="295"/>
+      <c r="E48" s="229"/>
+      <c r="F48" s="229"/>
+      <c r="G48" s="296"/>
     </row>
     <row r="49" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B49" s="289"/>
-      <c r="C49" s="289"/>
-      <c r="D49" s="296"/>
-      <c r="E49" s="248"/>
-      <c r="F49" s="248"/>
-      <c r="G49" s="297"/>
+      <c r="B49" s="308"/>
+      <c r="C49" s="308"/>
+      <c r="D49" s="295"/>
+      <c r="E49" s="229"/>
+      <c r="F49" s="229"/>
+      <c r="G49" s="296"/>
     </row>
     <row r="50" spans="2:7" ht="33.75" customHeight="1">
-      <c r="B50" s="290"/>
-      <c r="C50" s="290"/>
-      <c r="D50" s="298"/>
-      <c r="E50" s="299"/>
-      <c r="F50" s="299"/>
-      <c r="G50" s="300"/>
+      <c r="B50" s="309"/>
+      <c r="C50" s="309"/>
+      <c r="D50" s="297"/>
+      <c r="E50" s="298"/>
+      <c r="F50" s="298"/>
+      <c r="G50" s="299"/>
     </row>
     <row r="51" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B51" s="291" t="s">
+      <c r="B51" s="312" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="292" t="s">
+      <c r="C51" s="314" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="293" t="s">
+      <c r="D51" s="292" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="294"/>
-      <c r="F51" s="294"/>
-      <c r="G51" s="295"/>
+      <c r="E51" s="293"/>
+      <c r="F51" s="293"/>
+      <c r="G51" s="294"/>
     </row>
     <row r="52" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B52" s="289"/>
-      <c r="C52" s="289"/>
-      <c r="D52" s="296"/>
-      <c r="E52" s="248"/>
-      <c r="F52" s="248"/>
-      <c r="G52" s="297"/>
+      <c r="B52" s="308"/>
+      <c r="C52" s="308"/>
+      <c r="D52" s="295"/>
+      <c r="E52" s="229"/>
+      <c r="F52" s="229"/>
+      <c r="G52" s="296"/>
     </row>
     <row r="53" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B53" s="289"/>
-      <c r="C53" s="289"/>
-      <c r="D53" s="296"/>
-      <c r="E53" s="248"/>
-      <c r="F53" s="248"/>
-      <c r="G53" s="297"/>
+      <c r="B53" s="308"/>
+      <c r="C53" s="308"/>
+      <c r="D53" s="295"/>
+      <c r="E53" s="229"/>
+      <c r="F53" s="229"/>
+      <c r="G53" s="296"/>
     </row>
     <row r="54" spans="2:7" ht="39" customHeight="1">
-      <c r="B54" s="290"/>
-      <c r="C54" s="290"/>
-      <c r="D54" s="298"/>
-      <c r="E54" s="299"/>
-      <c r="F54" s="299"/>
-      <c r="G54" s="300"/>
+      <c r="B54" s="309"/>
+      <c r="C54" s="309"/>
+      <c r="D54" s="297"/>
+      <c r="E54" s="298"/>
+      <c r="F54" s="298"/>
+      <c r="G54" s="299"/>
     </row>
     <row r="55" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="56" spans="2:7" ht="15.75" customHeight="1"/>
@@ -16510,11 +16524,21 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:G50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:G54"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:G42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:G46"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="D27:G30"/>
@@ -16531,21 +16555,11 @@
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="B31:B34"/>
-    <mergeCell ref="D47:G50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:G54"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:G42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D43:G46"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>